<commit_message>
Revisi tanggal mulai dan akhir setiap tas
</commit_message>
<xml_diff>
--- a/Gantt onlinestss.com.xlsx
+++ b/Gantt onlinestss.com.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/discovery-air/Dropbox/Work/MUGI/SS/stssonline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Setiawan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0573CC68-F256-3244-957E-4FF92C15A41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="35960" windowHeight="21060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -29,7 +28,7 @@
     <definedName name="task_start" localSheetId="0">'Project schedule'!$K1</definedName>
     <definedName name="today" localSheetId="0">TODAY()</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,12 +49,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Theo Darmawan</author>
   </authors>
   <commentList>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{C55DF099-DB51-9143-89FE-70D53E3CEDA5}">
+    <comment ref="C11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{E0291CE9-D34C-6840-9E61-84ECC5186F27}">
+    <comment ref="C18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -122,7 +121,108 @@
         </r>
       </text>
     </comment>
-    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{B33F0D5A-58B4-164C-A431-1E03C312FF6B}">
+    <comment ref="C29" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Theo Darmawan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">set up lagi kalo pindah hosting
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C30" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Theo Darmawan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">pindah hosting hrs diulang
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C31" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Theo Darmawan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>jangan lupa merubah field / halaman sesuai tipe user</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C39" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -155,7 +255,108 @@
         </r>
       </text>
     </comment>
-    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{1D5D9DEA-CC0E-CA47-8A9A-55CE2229A885}">
+    <comment ref="C41" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Theo Darmawan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">sedang dicek apa daftar bisa diurutkan
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C48" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Theo Darmawan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">sudah jalan untuk user terbatas
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C57" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Theo Darmawan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">hrs set meeting sama keuangan, daftar pertanyaan terkait alur penjualan </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C59" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -189,214 +390,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="C30" authorId="0" shapeId="0" xr:uid="{E48CF6FD-3DE3-A742-9F80-48D6039EDD32}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Theo Darmawan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">pindah hosting hrs diulang
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C31" authorId="0" shapeId="0" xr:uid="{A0510CEC-6055-3F4B-966A-7D549003A848}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Theo Darmawan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>jangan lupa merubah field / halaman sesuai tipe user</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C37" authorId="0" shapeId="0" xr:uid="{D709CFE1-21F0-6C45-8EAD-651F34644C6F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Theo Darmawan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">hrs set meeting sama keuangan, daftar pertanyaan terkait alur penjualan </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C38" authorId="0" shapeId="0" xr:uid="{E1EA5362-C17C-E145-A97D-89ADFA73E599}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Theo Darmawan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">sudah jalan untuk user terbatas
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C48" authorId="0" shapeId="0" xr:uid="{DD682FC1-CE00-BE4E-B19E-30720D705022}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Theo Darmawan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">sedang dicek apa daftar bisa diurutkan
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C62" authorId="0" shapeId="0" xr:uid="{FD3E44BD-53F0-3E44-A49F-8EEBBFC75610}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Theo Darmawan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">set up lagi kalo pindah hosting
-</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="199">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -994,37 +993,16 @@
     <t>ES</t>
   </si>
   <si>
-    <t>ES,BP</t>
-  </si>
-  <si>
     <t>START (Actual)</t>
   </si>
   <si>
     <t>END (Actual)</t>
-  </si>
-  <si>
-    <t>2/26/25</t>
-  </si>
-  <si>
-    <t>2/27/25</t>
-  </si>
-  <si>
-    <t>5/15/25</t>
-  </si>
-  <si>
-    <t>6/18/25</t>
-  </si>
-  <si>
-    <t>6/19/25</t>
-  </si>
-  <si>
-    <t>6/23/25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
@@ -1032,7 +1010,7 @@
     <numFmt numFmtId="166" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="167" formatCode="d"/>
   </numFmts>
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="38">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1650,7 +1628,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1913,69 +1891,194 @@
     <xf numFmtId="0" fontId="30" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="11" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="11" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="11" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="11" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="12" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="20" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="20" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="19" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="19" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="19" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="20" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="19" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="20" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="19" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="19" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="19" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="20" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="4" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="5" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="20" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1984,15 +2087,37 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
+    <xf numFmtId="166" fontId="17" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2005,90 +2130,24 @@
     <xf numFmtId="0" fontId="18" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="12" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Date" xfId="10" xr:uid="{229918B6-DD13-4F5A-97B9-305F7E002AA3}"/>
+    <cellStyle name="Date" xfId="10"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="Name" xfId="11" xr:uid="{B2D3C1EE-6B41-4801-AAFC-C2274E49E503}"/>
+    <cellStyle name="Name" xfId="11"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
-    <cellStyle name="Project Start" xfId="9" xr:uid="{8EB8A09A-C31C-40A3-B2C1-9449520178B8}"/>
-    <cellStyle name="Task" xfId="12" xr:uid="{6391D789-272B-4DD2-9BF3-2CDCF610FA41}"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Project Start" xfId="9"/>
+    <cellStyle name="Task" xfId="12"/>
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
+    <cellStyle name="zHiddenText" xfId="3"/>
   </cellStyles>
   <dxfs count="16">
     <dxf>
@@ -2286,7 +2345,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="ToDoList" pivot="0" count="9">
       <tableStyleElement type="wholeTable" dxfId="15"/>
       <tableStyleElement type="headerRow" dxfId="14"/>
       <tableStyleElement type="totalRow" dxfId="13"/>
@@ -2410,7 +2469,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2651,41 +2710,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1" filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:EX74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="140" zoomScaleNormal="150" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="1" style="11" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" customWidth="1"/>
-    <col min="3" max="3" width="38.1640625" style="147" customWidth="1"/>
+    <col min="2" max="2" width="6.625" customWidth="1"/>
+    <col min="3" max="3" width="38.125" style="114" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="7" max="8" width="6.83203125" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" customWidth="1"/>
-    <col min="13" max="13" width="2.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.875" customWidth="1"/>
+    <col min="6" max="6" width="15.375" customWidth="1"/>
+    <col min="7" max="8" width="6.875" customWidth="1"/>
+    <col min="9" max="9" width="9.375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="7.625" customWidth="1"/>
+    <col min="11" max="11" width="9.375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="7.625" customWidth="1"/>
+    <col min="13" max="13" width="2.625" customWidth="1"/>
     <col min="14" max="14" width="6" hidden="1" customWidth="1"/>
-    <col min="15" max="38" width="2.6640625" customWidth="1"/>
-    <col min="39" max="39" width="6" customWidth="1"/>
-    <col min="40" max="154" width="2.6640625" customWidth="1"/>
+    <col min="15" max="38" width="2.625" customWidth="1"/>
+    <col min="39" max="39" width="2.375" bestFit="1" customWidth="1"/>
+    <col min="40" max="154" width="2.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:154" ht="74" customHeight="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:154" ht="74.099999999999994" customHeight="1">
       <c r="A1" s="12"/>
       <c r="B1" s="78"/>
-      <c r="C1" s="128" t="s">
+      <c r="C1" s="99" t="s">
         <v>54</v>
       </c>
       <c r="D1" s="78"/>
@@ -2698,52 +2757,52 @@
       <c r="K1" s="16"/>
       <c r="L1" s="21"/>
       <c r="N1" s="1"/>
-      <c r="O1" s="111" t="s">
+      <c r="O1" s="154" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="112"/>
-      <c r="Q1" s="112"/>
-      <c r="R1" s="112"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112"/>
-      <c r="U1" s="112"/>
+      <c r="P1" s="155"/>
+      <c r="Q1" s="155"/>
+      <c r="R1" s="155"/>
+      <c r="S1" s="155"/>
+      <c r="T1" s="155"/>
+      <c r="U1" s="155"/>
       <c r="V1" s="19"/>
-      <c r="W1" s="110">
+      <c r="W1" s="156">
         <v>45705</v>
       </c>
-      <c r="X1" s="109"/>
-      <c r="Y1" s="109"/>
-      <c r="Z1" s="109"/>
-      <c r="AA1" s="109"/>
-      <c r="AB1" s="109"/>
-      <c r="AC1" s="109"/>
-      <c r="AD1" s="109"/>
-      <c r="AE1" s="109"/>
-      <c r="AF1" s="109"/>
-      <c r="AG1" s="111" t="s">
+      <c r="X1" s="157"/>
+      <c r="Y1" s="157"/>
+      <c r="Z1" s="157"/>
+      <c r="AA1" s="157"/>
+      <c r="AB1" s="157"/>
+      <c r="AC1" s="157"/>
+      <c r="AD1" s="157"/>
+      <c r="AE1" s="157"/>
+      <c r="AF1" s="157"/>
+      <c r="AG1" s="154" t="s">
         <v>39</v>
       </c>
-      <c r="AH1" s="112"/>
-      <c r="AI1" s="112"/>
-      <c r="AJ1" s="112"/>
-      <c r="AK1" s="112"/>
-      <c r="AL1" s="112"/>
-      <c r="AM1" s="112"/>
+      <c r="AH1" s="155"/>
+      <c r="AI1" s="155"/>
+      <c r="AJ1" s="155"/>
+      <c r="AK1" s="155"/>
+      <c r="AL1" s="155"/>
+      <c r="AM1" s="155"/>
       <c r="AN1" s="19"/>
-      <c r="AO1" s="110">
+      <c r="AO1" s="156">
         <v>45838</v>
       </c>
-      <c r="AP1" s="109"/>
-      <c r="AQ1" s="109"/>
-      <c r="AR1" s="109"/>
-      <c r="AS1" s="109"/>
-      <c r="AT1" s="109"/>
-      <c r="AU1" s="109"/>
-      <c r="AV1" s="109"/>
-      <c r="AW1" s="109"/>
-      <c r="AX1" s="109"/>
+      <c r="AP1" s="157"/>
+      <c r="AQ1" s="157"/>
+      <c r="AR1" s="157"/>
+      <c r="AS1" s="157"/>
+      <c r="AT1" s="157"/>
+      <c r="AU1" s="157"/>
+      <c r="AV1" s="157"/>
+      <c r="AW1" s="157"/>
+      <c r="AX1" s="157"/>
     </row>
-    <row r="2" spans="1:154" ht="23" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:154" ht="23.1" customHeight="1">
       <c r="B2" s="66"/>
       <c r="C2" s="79" t="s">
         <v>19</v>
@@ -2753,307 +2812,307 @@
       </c>
       <c r="E2" s="18"/>
       <c r="F2" s="17"/>
-      <c r="O2" s="111" t="s">
+      <c r="O2" s="154" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="112"/>
-      <c r="Q2" s="112"/>
-      <c r="R2" s="112"/>
-      <c r="S2" s="112"/>
-      <c r="T2" s="112"/>
-      <c r="U2" s="112"/>
+      <c r="P2" s="155"/>
+      <c r="Q2" s="155"/>
+      <c r="R2" s="155"/>
+      <c r="S2" s="155"/>
+      <c r="T2" s="155"/>
+      <c r="U2" s="155"/>
       <c r="V2" s="19"/>
-      <c r="W2" s="108">
+      <c r="W2" s="165">
         <v>1</v>
       </c>
-      <c r="X2" s="109"/>
-      <c r="Y2" s="109"/>
-      <c r="Z2" s="109"/>
-      <c r="AA2" s="109"/>
-      <c r="AB2" s="109"/>
-      <c r="AC2" s="109"/>
-      <c r="AD2" s="109"/>
-      <c r="AE2" s="109"/>
-      <c r="AF2" s="109"/>
-      <c r="AG2" s="117" t="s">
+      <c r="X2" s="157"/>
+      <c r="Y2" s="157"/>
+      <c r="Z2" s="157"/>
+      <c r="AA2" s="157"/>
+      <c r="AB2" s="157"/>
+      <c r="AC2" s="157"/>
+      <c r="AD2" s="157"/>
+      <c r="AE2" s="157"/>
+      <c r="AF2" s="157"/>
+      <c r="AG2" s="158" t="s">
         <v>40</v>
       </c>
-      <c r="AH2" s="118"/>
-      <c r="AI2" s="118"/>
-      <c r="AJ2" s="118"/>
-      <c r="AK2" s="118"/>
-      <c r="AL2" s="118"/>
-      <c r="AM2" s="118"/>
+      <c r="AH2" s="159"/>
+      <c r="AI2" s="159"/>
+      <c r="AJ2" s="159"/>
+      <c r="AK2" s="159"/>
+      <c r="AL2" s="159"/>
+      <c r="AM2" s="159"/>
       <c r="AN2" s="19"/>
-      <c r="AO2" s="119">
+      <c r="AO2" s="160">
         <f ca="1">NETWORKDAYS(TODAY(),  Project_End, Holidays)</f>
-        <v>75</v>
-      </c>
-      <c r="AP2" s="120"/>
-      <c r="AQ2" s="120"/>
-      <c r="AR2" s="120"/>
-      <c r="AS2" s="120"/>
-      <c r="AT2" s="120"/>
-      <c r="AU2" s="120"/>
-      <c r="AV2" s="120"/>
-      <c r="AW2" s="120"/>
-      <c r="AX2" s="120"/>
+        <v>74</v>
+      </c>
+      <c r="AP2" s="161"/>
+      <c r="AQ2" s="161"/>
+      <c r="AR2" s="161"/>
+      <c r="AS2" s="161"/>
+      <c r="AT2" s="161"/>
+      <c r="AU2" s="161"/>
+      <c r="AV2" s="161"/>
+      <c r="AW2" s="161"/>
+      <c r="AX2" s="161"/>
     </row>
-    <row r="3" spans="1:154" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:154" s="21" customFormat="1" ht="21" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="20"/>
       <c r="C3" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="113" t="s">
+      <c r="D3" s="166" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="113"/>
-      <c r="F3" s="113"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="166"/>
     </row>
-    <row r="4" spans="1:154" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:154" s="21" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="12"/>
       <c r="B4" s="22"/>
-      <c r="C4" s="129"/>
+      <c r="C4" s="100"/>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
       <c r="F4" s="22"/>
       <c r="I4" s="23"/>
       <c r="K4" s="23"/>
-      <c r="O4" s="116">
+      <c r="O4" s="162">
         <f>O5</f>
         <v>45705</v>
       </c>
-      <c r="P4" s="114"/>
-      <c r="Q4" s="114"/>
-      <c r="R4" s="114"/>
-      <c r="S4" s="114"/>
-      <c r="T4" s="114"/>
-      <c r="U4" s="114"/>
-      <c r="V4" s="114">
+      <c r="P4" s="152"/>
+      <c r="Q4" s="152"/>
+      <c r="R4" s="152"/>
+      <c r="S4" s="152"/>
+      <c r="T4" s="152"/>
+      <c r="U4" s="152"/>
+      <c r="V4" s="152">
         <f>V5</f>
         <v>45712</v>
       </c>
-      <c r="W4" s="114"/>
-      <c r="X4" s="114"/>
-      <c r="Y4" s="114"/>
-      <c r="Z4" s="114"/>
-      <c r="AA4" s="114"/>
-      <c r="AB4" s="114"/>
-      <c r="AC4" s="114">
+      <c r="W4" s="152"/>
+      <c r="X4" s="152"/>
+      <c r="Y4" s="152"/>
+      <c r="Z4" s="152"/>
+      <c r="AA4" s="152"/>
+      <c r="AB4" s="152"/>
+      <c r="AC4" s="152">
         <f>AC5</f>
         <v>45719</v>
       </c>
-      <c r="AD4" s="114"/>
-      <c r="AE4" s="114"/>
-      <c r="AF4" s="114"/>
-      <c r="AG4" s="114"/>
-      <c r="AH4" s="114"/>
-      <c r="AI4" s="114"/>
-      <c r="AJ4" s="114">
+      <c r="AD4" s="152"/>
+      <c r="AE4" s="152"/>
+      <c r="AF4" s="152"/>
+      <c r="AG4" s="152"/>
+      <c r="AH4" s="152"/>
+      <c r="AI4" s="152"/>
+      <c r="AJ4" s="152">
         <f>AJ5</f>
         <v>45726</v>
       </c>
-      <c r="AK4" s="114"/>
-      <c r="AL4" s="114"/>
-      <c r="AM4" s="114"/>
-      <c r="AN4" s="114"/>
-      <c r="AO4" s="114"/>
-      <c r="AP4" s="114"/>
-      <c r="AQ4" s="114">
+      <c r="AK4" s="152"/>
+      <c r="AL4" s="152"/>
+      <c r="AM4" s="152"/>
+      <c r="AN4" s="152"/>
+      <c r="AO4" s="152"/>
+      <c r="AP4" s="152"/>
+      <c r="AQ4" s="152">
         <f>AQ5</f>
         <v>45733</v>
       </c>
-      <c r="AR4" s="114"/>
-      <c r="AS4" s="114"/>
-      <c r="AT4" s="114"/>
-      <c r="AU4" s="114"/>
-      <c r="AV4" s="114"/>
-      <c r="AW4" s="114"/>
-      <c r="AX4" s="114">
+      <c r="AR4" s="152"/>
+      <c r="AS4" s="152"/>
+      <c r="AT4" s="152"/>
+      <c r="AU4" s="152"/>
+      <c r="AV4" s="152"/>
+      <c r="AW4" s="152"/>
+      <c r="AX4" s="152">
         <f>AX5</f>
         <v>45740</v>
       </c>
-      <c r="AY4" s="114"/>
-      <c r="AZ4" s="114"/>
-      <c r="BA4" s="114"/>
-      <c r="BB4" s="114"/>
-      <c r="BC4" s="114"/>
-      <c r="BD4" s="114"/>
-      <c r="BE4" s="114">
+      <c r="AY4" s="152"/>
+      <c r="AZ4" s="152"/>
+      <c r="BA4" s="152"/>
+      <c r="BB4" s="152"/>
+      <c r="BC4" s="152"/>
+      <c r="BD4" s="152"/>
+      <c r="BE4" s="152">
         <f>BE5</f>
         <v>45747</v>
       </c>
-      <c r="BF4" s="114"/>
-      <c r="BG4" s="114"/>
-      <c r="BH4" s="114"/>
-      <c r="BI4" s="114"/>
-      <c r="BJ4" s="114"/>
-      <c r="BK4" s="114"/>
-      <c r="BL4" s="114">
+      <c r="BF4" s="152"/>
+      <c r="BG4" s="152"/>
+      <c r="BH4" s="152"/>
+      <c r="BI4" s="152"/>
+      <c r="BJ4" s="152"/>
+      <c r="BK4" s="152"/>
+      <c r="BL4" s="152">
         <f>BL5</f>
         <v>45754</v>
       </c>
-      <c r="BM4" s="114"/>
-      <c r="BN4" s="114"/>
-      <c r="BO4" s="114"/>
-      <c r="BP4" s="114"/>
-      <c r="BQ4" s="114"/>
-      <c r="BR4" s="115"/>
-      <c r="BS4" s="114">
+      <c r="BM4" s="152"/>
+      <c r="BN4" s="152"/>
+      <c r="BO4" s="152"/>
+      <c r="BP4" s="152"/>
+      <c r="BQ4" s="152"/>
+      <c r="BR4" s="153"/>
+      <c r="BS4" s="152">
         <f>BS5</f>
         <v>45761</v>
       </c>
-      <c r="BT4" s="114"/>
-      <c r="BU4" s="114"/>
-      <c r="BV4" s="114"/>
-      <c r="BW4" s="114"/>
-      <c r="BX4" s="114"/>
-      <c r="BY4" s="115"/>
-      <c r="BZ4" s="114">
+      <c r="BT4" s="152"/>
+      <c r="BU4" s="152"/>
+      <c r="BV4" s="152"/>
+      <c r="BW4" s="152"/>
+      <c r="BX4" s="152"/>
+      <c r="BY4" s="153"/>
+      <c r="BZ4" s="152">
         <f>BZ5</f>
         <v>45768</v>
       </c>
-      <c r="CA4" s="114"/>
-      <c r="CB4" s="114"/>
-      <c r="CC4" s="114"/>
-      <c r="CD4" s="114"/>
-      <c r="CE4" s="114"/>
-      <c r="CF4" s="115"/>
-      <c r="CG4" s="114">
+      <c r="CA4" s="152"/>
+      <c r="CB4" s="152"/>
+      <c r="CC4" s="152"/>
+      <c r="CD4" s="152"/>
+      <c r="CE4" s="152"/>
+      <c r="CF4" s="153"/>
+      <c r="CG4" s="152">
         <f>CG5</f>
         <v>45775</v>
       </c>
-      <c r="CH4" s="114"/>
-      <c r="CI4" s="114"/>
-      <c r="CJ4" s="114"/>
-      <c r="CK4" s="114"/>
-      <c r="CL4" s="114"/>
-      <c r="CM4" s="115"/>
-      <c r="CN4" s="114">
+      <c r="CH4" s="152"/>
+      <c r="CI4" s="152"/>
+      <c r="CJ4" s="152"/>
+      <c r="CK4" s="152"/>
+      <c r="CL4" s="152"/>
+      <c r="CM4" s="153"/>
+      <c r="CN4" s="152">
         <f>CN5</f>
         <v>45782</v>
       </c>
-      <c r="CO4" s="114"/>
-      <c r="CP4" s="114"/>
-      <c r="CQ4" s="114"/>
-      <c r="CR4" s="114"/>
-      <c r="CS4" s="114"/>
-      <c r="CT4" s="115"/>
-      <c r="CU4" s="114">
+      <c r="CO4" s="152"/>
+      <c r="CP4" s="152"/>
+      <c r="CQ4" s="152"/>
+      <c r="CR4" s="152"/>
+      <c r="CS4" s="152"/>
+      <c r="CT4" s="153"/>
+      <c r="CU4" s="152">
         <f>CU5</f>
         <v>45789</v>
       </c>
-      <c r="CV4" s="114"/>
-      <c r="CW4" s="114"/>
-      <c r="CX4" s="114"/>
-      <c r="CY4" s="114"/>
-      <c r="CZ4" s="114"/>
-      <c r="DA4" s="115"/>
-      <c r="DB4" s="114">
+      <c r="CV4" s="152"/>
+      <c r="CW4" s="152"/>
+      <c r="CX4" s="152"/>
+      <c r="CY4" s="152"/>
+      <c r="CZ4" s="152"/>
+      <c r="DA4" s="153"/>
+      <c r="DB4" s="152">
         <f>DB5</f>
         <v>45796</v>
       </c>
-      <c r="DC4" s="114"/>
-      <c r="DD4" s="114"/>
-      <c r="DE4" s="114"/>
-      <c r="DF4" s="114"/>
-      <c r="DG4" s="114"/>
-      <c r="DH4" s="115"/>
-      <c r="DI4" s="114">
+      <c r="DC4" s="152"/>
+      <c r="DD4" s="152"/>
+      <c r="DE4" s="152"/>
+      <c r="DF4" s="152"/>
+      <c r="DG4" s="152"/>
+      <c r="DH4" s="153"/>
+      <c r="DI4" s="152">
         <f>DI5</f>
         <v>45803</v>
       </c>
-      <c r="DJ4" s="114"/>
-      <c r="DK4" s="114"/>
-      <c r="DL4" s="114"/>
-      <c r="DM4" s="114"/>
-      <c r="DN4" s="114"/>
-      <c r="DO4" s="115"/>
-      <c r="DP4" s="114">
+      <c r="DJ4" s="152"/>
+      <c r="DK4" s="152"/>
+      <c r="DL4" s="152"/>
+      <c r="DM4" s="152"/>
+      <c r="DN4" s="152"/>
+      <c r="DO4" s="153"/>
+      <c r="DP4" s="152">
         <f>DP5</f>
         <v>45810</v>
       </c>
-      <c r="DQ4" s="114"/>
-      <c r="DR4" s="114"/>
-      <c r="DS4" s="114"/>
-      <c r="DT4" s="114"/>
-      <c r="DU4" s="114"/>
-      <c r="DV4" s="115"/>
-      <c r="DW4" s="114">
+      <c r="DQ4" s="152"/>
+      <c r="DR4" s="152"/>
+      <c r="DS4" s="152"/>
+      <c r="DT4" s="152"/>
+      <c r="DU4" s="152"/>
+      <c r="DV4" s="153"/>
+      <c r="DW4" s="152">
         <f>DW5</f>
         <v>45817</v>
       </c>
-      <c r="DX4" s="114"/>
-      <c r="DY4" s="114"/>
-      <c r="DZ4" s="114"/>
-      <c r="EA4" s="114"/>
-      <c r="EB4" s="114"/>
-      <c r="EC4" s="115"/>
-      <c r="ED4" s="114">
+      <c r="DX4" s="152"/>
+      <c r="DY4" s="152"/>
+      <c r="DZ4" s="152"/>
+      <c r="EA4" s="152"/>
+      <c r="EB4" s="152"/>
+      <c r="EC4" s="153"/>
+      <c r="ED4" s="152">
         <f>ED5</f>
         <v>45824</v>
       </c>
-      <c r="EE4" s="114"/>
-      <c r="EF4" s="114"/>
-      <c r="EG4" s="114"/>
-      <c r="EH4" s="114"/>
-      <c r="EI4" s="114"/>
-      <c r="EJ4" s="115"/>
-      <c r="EK4" s="114">
+      <c r="EE4" s="152"/>
+      <c r="EF4" s="152"/>
+      <c r="EG4" s="152"/>
+      <c r="EH4" s="152"/>
+      <c r="EI4" s="152"/>
+      <c r="EJ4" s="153"/>
+      <c r="EK4" s="152">
         <f>EK5</f>
         <v>45831</v>
       </c>
-      <c r="EL4" s="114"/>
-      <c r="EM4" s="114"/>
-      <c r="EN4" s="114"/>
-      <c r="EO4" s="114"/>
-      <c r="EP4" s="114"/>
-      <c r="EQ4" s="115"/>
-      <c r="ER4" s="114">
+      <c r="EL4" s="152"/>
+      <c r="EM4" s="152"/>
+      <c r="EN4" s="152"/>
+      <c r="EO4" s="152"/>
+      <c r="EP4" s="152"/>
+      <c r="EQ4" s="153"/>
+      <c r="ER4" s="152">
         <f>ER5</f>
         <v>45838</v>
       </c>
-      <c r="ES4" s="114"/>
-      <c r="ET4" s="114"/>
-      <c r="EU4" s="114"/>
-      <c r="EV4" s="114"/>
-      <c r="EW4" s="114"/>
-      <c r="EX4" s="115"/>
+      <c r="ES4" s="152"/>
+      <c r="ET4" s="152"/>
+      <c r="EU4" s="152"/>
+      <c r="EV4" s="152"/>
+      <c r="EW4" s="152"/>
+      <c r="EX4" s="153"/>
     </row>
-    <row r="5" spans="1:154" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="102"/>
-      <c r="B5" s="126" t="s">
+    <row r="5" spans="1:154" s="21" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A5" s="167"/>
+      <c r="B5" s="175" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="130" t="s">
+      <c r="C5" s="168" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="124" t="s">
+      <c r="D5" s="173" t="s">
         <v>116</v>
       </c>
-      <c r="E5" s="105" t="s">
+      <c r="E5" s="163" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="105" t="s">
+      <c r="F5" s="163" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="103" t="s">
+      <c r="G5" s="170" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="105" t="s">
+      <c r="H5" s="163" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="126" t="s">
+      <c r="I5" s="175" t="s">
+        <v>197</v>
+      </c>
+      <c r="J5" s="175" t="s">
         <v>198</v>
       </c>
-      <c r="J5" s="126" t="s">
-        <v>199</v>
-      </c>
-      <c r="K5" s="105" t="s">
+      <c r="K5" s="163" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="105" t="s">
+      <c r="L5" s="163" t="s">
         <v>4</v>
       </c>
       <c r="O5" s="24">
@@ -3617,19 +3676,19 @@
         <v>45844</v>
       </c>
     </row>
-    <row r="6" spans="1:154" s="21" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="102"/>
-      <c r="B6" s="127"/>
-      <c r="C6" s="131"/>
-      <c r="D6" s="125"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="107"/>
-      <c r="G6" s="104"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="149"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="106"/>
-      <c r="L6" s="107"/>
+    <row r="6" spans="1:154" s="21" customFormat="1" ht="15" hidden="1" customHeight="1" thickBot="1">
+      <c r="A6" s="167"/>
+      <c r="B6" s="176"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="174"/>
+      <c r="E6" s="164"/>
+      <c r="F6" s="164"/>
+      <c r="G6" s="171"/>
+      <c r="H6" s="172"/>
+      <c r="I6" s="177"/>
+      <c r="J6" s="176"/>
+      <c r="K6" s="172"/>
+      <c r="L6" s="164"/>
       <c r="O6" s="27" t="str">
         <f t="shared" ref="O6:AT6" si="63">LEFT(TEXT(O5,"ddd"),1)</f>
         <v>M</v>
@@ -4191,10 +4250,10 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A7" s="12"/>
       <c r="B7" s="83"/>
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="101" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="83"/>
@@ -4352,12 +4411,12 @@
       <c r="EW7" s="32"/>
       <c r="EX7" s="32"/>
     </row>
-    <row r="8" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A8" s="12"/>
       <c r="B8" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="133" t="s">
+      <c r="C8" s="102" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="34"/>
@@ -4387,8 +4446,8 @@
       <c r="L8" s="37">
         <v>45709</v>
       </c>
-      <c r="M8" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L8, H8&lt;1), -1, IF(H8=1, 1, 0))</f>
+      <c r="M8" s="115">
+        <f t="shared" ref="M8:M16" ca="1" si="69">IF(AND(TODAY()&gt;L8, H8&lt;1), -1, IF(H8=1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="N8" s="3">
@@ -4536,12 +4595,12 @@
       <c r="EW8" s="38"/>
       <c r="EX8" s="38"/>
     </row>
-    <row r="9" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A9" s="12"/>
       <c r="B9" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="134" t="s">
+      <c r="C9" s="103" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="34"/>
@@ -4566,8 +4625,8 @@
       <c r="L9" s="37">
         <v>45709</v>
       </c>
-      <c r="M9" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L9, H9&lt;1), -1, IF(H9=1, 1, 0))</f>
+      <c r="M9" s="115">
+        <f t="shared" ca="1" si="69"/>
         <v>-1</v>
       </c>
       <c r="N9" s="3">
@@ -4715,12 +4774,12 @@
       <c r="EW9" s="38"/>
       <c r="EX9" s="38"/>
     </row>
-    <row r="10" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A10" s="11"/>
       <c r="B10" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="134" t="s">
+      <c r="C10" s="103" t="s">
         <v>110</v>
       </c>
       <c r="D10" s="34"/>
@@ -4736,19 +4795,15 @@
       <c r="H10" s="40">
         <v>0</v>
       </c>
-      <c r="I10" s="150" t="s">
-        <v>200</v>
-      </c>
-      <c r="J10" s="150" t="s">
-        <v>201</v>
-      </c>
+      <c r="I10" s="116"/>
+      <c r="J10" s="116"/>
       <c r="K10" s="37">
         <v>45712</v>
       </c>
       <c r="L10" s="37">
         <v>45719</v>
       </c>
-      <c r="M10" s="148">
+      <c r="M10" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L10, H10&lt;1), -1, IF(H10=1, 1, 0))</f>
         <v>0</v>
       </c>
@@ -4897,12 +4952,12 @@
       <c r="EW10" s="38"/>
       <c r="EX10" s="38"/>
     </row>
-    <row r="11" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A11" s="11"/>
       <c r="B11" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="C11" s="134" t="s">
+      <c r="C11" s="103" t="s">
         <v>99</v>
       </c>
       <c r="D11" s="34"/>
@@ -4926,8 +4981,8 @@
       <c r="L11" s="41">
         <v>45808</v>
       </c>
-      <c r="M11" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L11, H11&lt;1), -1, IF(H11=1, 1, 0))</f>
+      <c r="M11" s="115">
+        <f t="shared" ca="1" si="69"/>
         <v>0</v>
       </c>
       <c r="N11" s="3">
@@ -5075,12 +5130,12 @@
       <c r="EW11" s="38"/>
       <c r="EX11" s="38"/>
     </row>
-    <row r="12" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A12" s="11"/>
       <c r="B12" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="134" t="s">
+      <c r="C12" s="103" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="34"/>
@@ -5110,8 +5165,8 @@
       <c r="L12" s="37">
         <v>45709</v>
       </c>
-      <c r="M12" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L12, H12&lt;1), -1, IF(H12=1, 1, 0))</f>
+      <c r="M12" s="115">
+        <f t="shared" ca="1" si="69"/>
         <v>1</v>
       </c>
       <c r="N12" s="3">
@@ -5259,12 +5314,12 @@
       <c r="EW12" s="38"/>
       <c r="EX12" s="38"/>
     </row>
-    <row r="13" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A13" s="11"/>
       <c r="B13" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="C13" s="134" t="s">
+      <c r="C13" s="103" t="s">
         <v>35</v>
       </c>
       <c r="D13" s="34"/>
@@ -5294,8 +5349,8 @@
       <c r="L13" s="41">
         <v>45709</v>
       </c>
-      <c r="M13" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L13, H13&lt;1), -1, IF(H13=1, 1, 0))</f>
+      <c r="M13" s="115">
+        <f t="shared" ca="1" si="69"/>
         <v>1</v>
       </c>
       <c r="N13" s="3">
@@ -5443,12 +5498,12 @@
       <c r="EW13" s="38"/>
       <c r="EX13" s="38"/>
     </row>
-    <row r="14" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A14" s="11"/>
       <c r="B14" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="C14" s="134" t="s">
+      <c r="C14" s="103" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="34"/>
@@ -5478,8 +5533,8 @@
       <c r="L14" s="37">
         <v>45709</v>
       </c>
-      <c r="M14" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L14, H14&lt;1), -1, IF(H14=1, 1, 0))</f>
+      <c r="M14" s="115">
+        <f t="shared" ca="1" si="69"/>
         <v>1</v>
       </c>
       <c r="N14" s="3"/>
@@ -5624,12 +5679,12 @@
       <c r="EW14" s="38"/>
       <c r="EX14" s="38"/>
     </row>
-    <row r="15" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A15" s="11"/>
       <c r="B15" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="C15" s="134" t="s">
+      <c r="C15" s="103" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="34"/>
@@ -5659,8 +5714,8 @@
       <c r="L15" s="37">
         <v>45709</v>
       </c>
-      <c r="M15" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L15, H15&lt;1), -1, IF(H15=1, 1, 0))</f>
+      <c r="M15" s="115">
+        <f t="shared" ca="1" si="69"/>
         <v>1</v>
       </c>
       <c r="N15" s="3"/>
@@ -5805,12 +5860,12 @@
       <c r="EW15" s="38"/>
       <c r="EX15" s="38"/>
     </row>
-    <row r="16" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A16" s="11"/>
       <c r="B16" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="C16" s="134" t="s">
+      <c r="C16" s="103" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="34"/>
@@ -5840,8 +5895,8 @@
       <c r="L16" s="37">
         <v>45709</v>
       </c>
-      <c r="M16" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L16, H16&lt;1), -1, IF(H16=1, 1, 0))</f>
+      <c r="M16" s="115">
+        <f t="shared" ca="1" si="69"/>
         <v>1</v>
       </c>
       <c r="N16" s="3"/>
@@ -5986,13 +6041,13 @@
       <c r="EW16" s="38"/>
       <c r="EX16" s="38"/>
     </row>
-    <row r="17" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A17" s="11"/>
       <c r="B17" s="34"/>
-      <c r="C17" s="135" t="s">
+      <c r="C17" s="104" t="s">
         <v>95</v>
       </c>
-      <c r="D17" s="121"/>
+      <c r="D17" s="96"/>
       <c r="E17" s="34"/>
       <c r="F17" s="34"/>
       <c r="G17" s="39"/>
@@ -6001,7 +6056,7 @@
       <c r="J17" s="37"/>
       <c r="K17" s="37"/>
       <c r="L17" s="37"/>
-      <c r="M17" s="148"/>
+      <c r="M17" s="115"/>
       <c r="N17" s="3"/>
       <c r="O17" s="38"/>
       <c r="P17" s="38"/>
@@ -6144,15 +6199,15 @@
       <c r="EW17" s="38"/>
       <c r="EX17" s="38"/>
     </row>
-    <row r="18" spans="1:154" s="33" customFormat="1" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:154" s="33" customFormat="1" ht="36.950000000000003" hidden="1" customHeight="1" thickBot="1">
       <c r="A18" s="11"/>
       <c r="B18" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="C18" s="136" t="s">
+      <c r="C18" s="105" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="122"/>
+      <c r="D18" s="97"/>
       <c r="E18" s="34" t="s">
         <v>71</v>
       </c>
@@ -6177,7 +6232,7 @@
       <c r="L18" s="37">
         <v>45716</v>
       </c>
-      <c r="M18" s="148">
+      <c r="M18" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L18, H18&lt;1), -1, IF(H18=1, 1, 0))</f>
         <v>0</v>
       </c>
@@ -6323,15 +6378,15 @@
       <c r="EW18" s="38"/>
       <c r="EX18" s="38"/>
     </row>
-    <row r="19" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A19" s="11"/>
       <c r="B19" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="C19" s="136" t="s">
+      <c r="C19" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="122"/>
+      <c r="D19" s="97"/>
       <c r="E19" s="34" t="s">
         <v>33</v>
       </c>
@@ -6356,7 +6411,7 @@
       <c r="L19" s="37">
         <v>45709</v>
       </c>
-      <c r="M19" s="148">
+      <c r="M19" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L19, H19&lt;1), -1, IF(H19=1, 1, 0))</f>
         <v>-1</v>
       </c>
@@ -6502,42 +6557,42 @@
       <c r="EW19" s="38"/>
       <c r="EX19" s="38"/>
     </row>
-    <row r="20" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A20" s="11"/>
-      <c r="B20" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="C20" s="136" t="s">
-        <v>94</v>
-      </c>
-      <c r="D20" s="123"/>
-      <c r="E20" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="G20" s="39" t="s">
+      <c r="B20" s="117" t="s">
+        <v>144</v>
+      </c>
+      <c r="C20" s="145" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="146"/>
+      <c r="E20" s="147" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="147" t="s">
+        <v>96</v>
+      </c>
+      <c r="G20" s="133" t="s">
         <v>196</v>
       </c>
-      <c r="H20" s="40">
-        <v>0</v>
-      </c>
-      <c r="I20" s="37">
-        <v>45740</v>
-      </c>
-      <c r="J20" s="37">
-        <v>45744</v>
-      </c>
-      <c r="K20" s="37">
-        <v>45707</v>
-      </c>
-      <c r="L20" s="37">
-        <v>45735</v>
-      </c>
-      <c r="M20" s="148">
+      <c r="H20" s="149">
+        <v>1</v>
+      </c>
+      <c r="I20" s="150">
+        <v>45705</v>
+      </c>
+      <c r="J20" s="150">
+        <v>45709</v>
+      </c>
+      <c r="K20" s="48">
+        <v>45705</v>
+      </c>
+      <c r="L20" s="48">
+        <v>45709</v>
+      </c>
+      <c r="M20" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L20, H20&lt;1), -1, IF(H20=1, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="38"/>
@@ -6681,42 +6736,42 @@
       <c r="EW20" s="38"/>
       <c r="EX20" s="38"/>
     </row>
-    <row r="21" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A21" s="11"/>
-      <c r="B21" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="C21" s="136" t="s">
-        <v>104</v>
-      </c>
-      <c r="D21" s="123"/>
-      <c r="E21" s="34" t="s">
+      <c r="B21" s="146" t="s">
+        <v>150</v>
+      </c>
+      <c r="C21" s="145" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="146"/>
+      <c r="E21" s="147" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="G21" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="H21" s="40">
-        <v>0</v>
-      </c>
-      <c r="I21" s="37">
-        <v>45784</v>
-      </c>
-      <c r="J21" s="37">
-        <v>45791</v>
-      </c>
-      <c r="K21" s="37">
-        <v>45712</v>
-      </c>
-      <c r="L21" s="37">
-        <v>45721</v>
-      </c>
-      <c r="M21" s="148">
+      <c r="F21" s="129" t="s">
+        <v>103</v>
+      </c>
+      <c r="G21" s="148" t="s">
+        <v>196</v>
+      </c>
+      <c r="H21" s="149">
+        <v>1</v>
+      </c>
+      <c r="I21" s="150">
+        <v>45710</v>
+      </c>
+      <c r="J21" s="150">
+        <v>45711</v>
+      </c>
+      <c r="K21" s="150">
+        <v>45710</v>
+      </c>
+      <c r="L21" s="150">
+        <v>45711</v>
+      </c>
+      <c r="M21" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L21, H21&lt;1), -1, IF(H21=1, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21" s="3"/>
       <c r="O21" s="38"/>
@@ -6860,15 +6915,15 @@
       <c r="EW21" s="38"/>
       <c r="EX21" s="38"/>
     </row>
-    <row r="22" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A22" s="11"/>
       <c r="B22" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="C22" s="136" t="s">
+      <c r="C22" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="123"/>
+      <c r="D22" s="98"/>
       <c r="E22" s="34" t="s">
         <v>97</v>
       </c>
@@ -6893,7 +6948,7 @@
       <c r="L22" s="37">
         <v>45730</v>
       </c>
-      <c r="M22" s="148">
+      <c r="M22" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L22, H22&lt;1), -1, IF(H22=1, 1, 0))</f>
         <v>0</v>
       </c>
@@ -7039,13 +7094,13 @@
       <c r="EW22" s="38"/>
       <c r="EX22" s="38"/>
     </row>
-    <row r="23" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A23" s="11"/>
       <c r="B23" s="34"/>
-      <c r="C23" s="137" t="s">
+      <c r="C23" s="106" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="123"/>
+      <c r="D23" s="98"/>
       <c r="E23" s="34"/>
       <c r="F23" s="34"/>
       <c r="G23" s="39"/>
@@ -7054,7 +7109,7 @@
       <c r="J23" s="37"/>
       <c r="K23" s="37"/>
       <c r="L23" s="37"/>
-      <c r="M23" s="148"/>
+      <c r="M23" s="115"/>
       <c r="N23" s="3"/>
       <c r="O23" s="38"/>
       <c r="P23" s="38"/>
@@ -7197,15 +7252,15 @@
       <c r="EW23" s="38"/>
       <c r="EX23" s="38"/>
     </row>
-    <row r="24" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A24" s="11"/>
       <c r="B24" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="C24" s="136" t="s">
+      <c r="C24" s="105" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="123"/>
+      <c r="D24" s="98"/>
       <c r="E24" s="34" t="s">
         <v>60</v>
       </c>
@@ -7218,19 +7273,15 @@
       <c r="H24" s="40">
         <v>0</v>
       </c>
-      <c r="I24" s="37">
-        <v>45748</v>
-      </c>
-      <c r="J24" s="37">
-        <v>45809</v>
-      </c>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
       <c r="K24" s="37">
         <v>45712</v>
       </c>
       <c r="L24" s="37">
         <v>45714</v>
       </c>
-      <c r="M24" s="148">
+      <c r="M24" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L24, H24&lt;1), -1, IF(H24=1, 1, 0))</f>
         <v>0</v>
       </c>
@@ -7376,15 +7427,15 @@
       <c r="EW24" s="38"/>
       <c r="EX24" s="38"/>
     </row>
-    <row r="25" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A25" s="11"/>
       <c r="B25" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="C25" s="136" t="s">
+      <c r="C25" s="105" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="123"/>
+      <c r="D25" s="98"/>
       <c r="E25" s="34" t="s">
         <v>60</v>
       </c>
@@ -7397,19 +7448,15 @@
       <c r="H25" s="40">
         <v>0</v>
       </c>
-      <c r="I25" s="37">
-        <v>45748</v>
-      </c>
-      <c r="J25" s="37">
-        <v>45809</v>
-      </c>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
       <c r="K25" s="37">
         <v>45712</v>
       </c>
       <c r="L25" s="37">
         <v>45714</v>
       </c>
-      <c r="M25" s="148">
+      <c r="M25" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L25, H25&lt;1), -1, IF(H25=1, 1, 0))</f>
         <v>0</v>
       </c>
@@ -7555,15 +7602,15 @@
       <c r="EW25" s="38"/>
       <c r="EX25" s="38"/>
     </row>
-    <row r="26" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A26" s="11"/>
       <c r="B26" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="C26" s="136" t="s">
+      <c r="C26" s="105" t="s">
         <v>93</v>
       </c>
-      <c r="D26" s="123"/>
+      <c r="D26" s="98"/>
       <c r="E26" s="34" t="s">
         <v>60</v>
       </c>
@@ -7576,19 +7623,15 @@
       <c r="H26" s="40">
         <v>0</v>
       </c>
-      <c r="I26" s="37">
-        <v>45748</v>
-      </c>
-      <c r="J26" s="37">
-        <v>45809</v>
-      </c>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
       <c r="K26" s="37">
         <v>45712</v>
       </c>
       <c r="L26" s="37">
         <v>45714</v>
       </c>
-      <c r="M26" s="148">
+      <c r="M26" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L26, H26&lt;1), -1, IF(H26=1, 1, 0))</f>
         <v>0</v>
       </c>
@@ -7737,10 +7780,10 @@
       <c r="EW26" s="38"/>
       <c r="EX26" s="38"/>
     </row>
-    <row r="27" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A27" s="12"/>
       <c r="B27" s="85"/>
-      <c r="C27" s="138" t="s">
+      <c r="C27" s="107" t="s">
         <v>59</v>
       </c>
       <c r="D27" s="85"/>
@@ -7752,19 +7795,19 @@
       <c r="J27" s="91"/>
       <c r="K27" s="88"/>
       <c r="L27" s="91"/>
-      <c r="M27" s="148"/>
+      <c r="M27" s="115"/>
       <c r="N27" s="3" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A28" s="12"/>
-      <c r="B28" s="101"/>
-      <c r="C28" s="139" t="s">
+      <c r="B28" s="95"/>
+      <c r="C28" s="108" t="s">
         <v>194</v>
       </c>
-      <c r="D28" s="101"/>
+      <c r="D28" s="95"/>
       <c r="E28" s="45"/>
       <c r="F28" s="45"/>
       <c r="G28" s="46"/>
@@ -7773,7 +7816,7 @@
       <c r="J28" s="48"/>
       <c r="K28" s="48"/>
       <c r="L28" s="48"/>
-      <c r="M28" s="148"/>
+      <c r="M28" s="115"/>
       <c r="N28" s="3" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
@@ -7919,22 +7962,22 @@
       <c r="EW28" s="38"/>
       <c r="EX28" s="38"/>
     </row>
-    <row r="29" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A29" s="12"/>
-      <c r="B29" s="80" t="s">
-        <v>138</v>
-      </c>
-      <c r="C29" s="140" t="s">
-        <v>111</v>
+      <c r="B29" s="94" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29" s="109" t="s">
+        <v>67</v>
       </c>
       <c r="D29" s="80" t="s">
-        <v>130</v>
+        <v>184</v>
       </c>
       <c r="E29" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="F29" s="81" t="s">
-        <v>103</v>
+        <v>70</v>
+      </c>
+      <c r="F29" s="130" t="s">
+        <v>87</v>
       </c>
       <c r="G29" s="46" t="s">
         <v>196</v>
@@ -7944,13 +7987,13 @@
       </c>
       <c r="I29" s="48"/>
       <c r="J29" s="48"/>
-      <c r="K29" s="48" t="s">
-        <v>202</v>
-      </c>
-      <c r="L29" s="48" t="s">
-        <v>203</v>
-      </c>
-      <c r="M29" s="148">
+      <c r="K29" s="48">
+        <v>45712</v>
+      </c>
+      <c r="L29" s="48">
+        <v>45714</v>
+      </c>
+      <c r="M29" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L29, H29&lt;1), -1, IF(H29=1, 1, 0))</f>
         <v>0</v>
       </c>
@@ -8096,12 +8139,12 @@
       <c r="EW29" s="38"/>
       <c r="EX29" s="38"/>
     </row>
-    <row r="30" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A30" s="12"/>
       <c r="B30" s="80" t="s">
         <v>139</v>
       </c>
-      <c r="C30" s="140" t="s">
+      <c r="C30" s="109" t="s">
         <v>107</v>
       </c>
       <c r="D30" s="80" t="s">
@@ -8125,9 +8168,9 @@
         <v>45712</v>
       </c>
       <c r="L30" s="48">
-        <v>45713</v>
-      </c>
-      <c r="M30" s="148">
+        <v>45714</v>
+      </c>
+      <c r="M30" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L30, H30&lt;1), -1, IF(H30=1, 1, 0))</f>
         <v>0</v>
       </c>
@@ -8273,12 +8316,12 @@
       <c r="EW30" s="38"/>
       <c r="EX30" s="38"/>
     </row>
-    <row r="31" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A31" s="12"/>
       <c r="B31" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="140" t="s">
+      <c r="C31" s="109" t="s">
         <v>178</v>
       </c>
       <c r="D31" s="80"/>
@@ -8302,7 +8345,7 @@
       <c r="L31" s="48">
         <v>45716</v>
       </c>
-      <c r="M31" s="148">
+      <c r="M31" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L31, H31&lt;1), -1, IF(H31=1, 1, 0))</f>
         <v>0</v>
       </c>
@@ -8448,22 +8491,22 @@
       <c r="EW31" s="38"/>
       <c r="EX31" s="38"/>
     </row>
-    <row r="32" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A32" s="12"/>
-      <c r="B32" s="80" t="s">
-        <v>141</v>
-      </c>
-      <c r="C32" s="140" t="s">
-        <v>106</v>
+      <c r="B32" s="119" t="s">
+        <v>148</v>
+      </c>
+      <c r="C32" s="109" t="s">
+        <v>51</v>
       </c>
       <c r="D32" s="80"/>
       <c r="E32" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="F32" s="81" t="s">
-        <v>103</v>
-      </c>
-      <c r="G32" s="46" t="s">
+      <c r="F32" s="130" t="s">
+        <v>96</v>
+      </c>
+      <c r="G32" s="135" t="s">
         <v>196</v>
       </c>
       <c r="H32" s="47">
@@ -8472,12 +8515,12 @@
       <c r="I32" s="48"/>
       <c r="J32" s="48"/>
       <c r="K32" s="48">
-        <v>45762</v>
+        <v>45714</v>
       </c>
       <c r="L32" s="48">
-        <v>45763</v>
-      </c>
-      <c r="M32" s="148">
+        <v>45716</v>
+      </c>
+      <c r="M32" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L32, H32&lt;1), -1, IF(H32=1, 1, 0))</f>
         <v>0</v>
       </c>
@@ -8623,13 +8666,13 @@
       <c r="EW32" s="38"/>
       <c r="EX32" s="38"/>
     </row>
-    <row r="33" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A33" s="12"/>
-      <c r="B33" s="101"/>
-      <c r="C33" s="139" t="s">
+      <c r="B33" s="95"/>
+      <c r="C33" s="108" t="s">
         <v>193</v>
       </c>
-      <c r="D33" s="101"/>
+      <c r="D33" s="95"/>
       <c r="E33" s="45"/>
       <c r="F33" s="45"/>
       <c r="G33" s="46"/>
@@ -8638,7 +8681,7 @@
       <c r="J33" s="48"/>
       <c r="K33" s="48"/>
       <c r="L33" s="48"/>
-      <c r="M33" s="148"/>
+      <c r="M33" s="115"/>
       <c r="N33" s="3" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
@@ -8784,39 +8827,37 @@
       <c r="EW33" s="38"/>
       <c r="EX33" s="38"/>
     </row>
-    <row r="34" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A34" s="12"/>
       <c r="B34" s="92" t="s">
-        <v>142</v>
-      </c>
-      <c r="C34" s="141" t="s">
-        <v>179</v>
-      </c>
-      <c r="D34" s="92" t="s">
-        <v>181</v>
-      </c>
-      <c r="E34" s="81" t="s">
-        <v>74</v>
-      </c>
-      <c r="F34" s="81" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" s="124" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="122"/>
+      <c r="E34" s="130" t="s">
+        <v>70</v>
+      </c>
+      <c r="F34" s="130" t="s">
         <v>96</v>
       </c>
       <c r="G34" s="93" t="s">
         <v>196</v>
       </c>
-      <c r="H34" s="94">
+      <c r="H34" s="137">
         <v>0</v>
       </c>
-      <c r="I34" s="95"/>
-      <c r="J34" s="95"/>
-      <c r="K34" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="L34" s="95" t="s">
-        <v>205</v>
-      </c>
-      <c r="M34" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L34, H34&lt;1), -1, IF(H34=1, 1, 0))</f>
+      <c r="I34" s="141"/>
+      <c r="J34" s="141"/>
+      <c r="K34" s="48">
+        <v>45719</v>
+      </c>
+      <c r="L34" s="48">
+        <v>45721</v>
+      </c>
+      <c r="M34" s="115">
+        <f t="shared" ref="M34:M41" ca="1" si="70">IF(AND(TODAY()&gt;L34, H34&lt;1), -1, IF(H34=1, 1, 0))</f>
         <v>0</v>
       </c>
       <c r="N34" s="3"/>
@@ -8961,39 +9002,37 @@
       <c r="EW34" s="38"/>
       <c r="EX34" s="38"/>
     </row>
-    <row r="35" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A35" s="12"/>
-      <c r="B35" s="96" t="s">
-        <v>143</v>
-      </c>
-      <c r="C35" s="142" t="s">
-        <v>180</v>
-      </c>
-      <c r="D35" s="96" t="s">
-        <v>181</v>
-      </c>
-      <c r="E35" s="97" t="s">
-        <v>72</v>
-      </c>
-      <c r="F35" s="97" t="s">
-        <v>96</v>
+      <c r="B35" s="120" t="s">
+        <v>159</v>
+      </c>
+      <c r="C35" s="126" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="120"/>
+      <c r="E35" s="132" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35" s="132" t="s">
+        <v>87</v>
       </c>
       <c r="G35" s="93" t="s">
         <v>196</v>
       </c>
-      <c r="H35" s="98">
+      <c r="H35" s="139">
         <v>0</v>
       </c>
-      <c r="I35" s="99"/>
-      <c r="J35" s="99"/>
-      <c r="K35" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="L35" s="95" t="s">
-        <v>205</v>
-      </c>
-      <c r="M35" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L35, H35&lt;1), -1, IF(H35=1, 1, 0))</f>
+      <c r="I35" s="143"/>
+      <c r="J35" s="143"/>
+      <c r="K35" s="48">
+        <v>45722</v>
+      </c>
+      <c r="L35" s="48">
+        <v>45727</v>
+      </c>
+      <c r="M35" s="115">
+        <f t="shared" ca="1" si="70"/>
         <v>0</v>
       </c>
       <c r="N35" s="3"/>
@@ -9138,46 +9177,42 @@
       <c r="EW35" s="38"/>
       <c r="EX35" s="38"/>
     </row>
-    <row r="36" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A36" s="12"/>
-      <c r="B36" s="92" t="s">
-        <v>144</v>
-      </c>
-      <c r="C36" s="140" t="s">
-        <v>41</v>
+      <c r="B36" s="123" t="s">
+        <v>160</v>
+      </c>
+      <c r="C36" s="109" t="s">
+        <v>186</v>
       </c>
       <c r="D36" s="80"/>
       <c r="E36" s="45" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="F36" s="45" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G36" s="93" t="s">
         <v>196</v>
       </c>
       <c r="H36" s="47">
-        <v>1</v>
-      </c>
-      <c r="I36" s="48">
-        <v>45705</v>
-      </c>
-      <c r="J36" s="48">
-        <v>45709</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
       <c r="K36" s="48">
-        <v>45714</v>
+        <v>45727</v>
       </c>
       <c r="L36" s="48">
-        <v>45716</v>
-      </c>
-      <c r="M36" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L36, H36&lt;1), -1, IF(H36=1, 1, 0))</f>
-        <v>1</v>
+        <v>45737</v>
+      </c>
+      <c r="M36" s="115">
+        <f t="shared" ca="1" si="70"/>
+        <v>0</v>
       </c>
       <c r="N36" s="3">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="O36" s="38"/>
       <c r="P36" s="38"/>
@@ -9320,22 +9355,20 @@
       <c r="EW36" s="38"/>
       <c r="EX36" s="38"/>
     </row>
-    <row r="37" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A37" s="12"/>
-      <c r="B37" s="96" t="s">
-        <v>145</v>
-      </c>
-      <c r="C37" s="140" t="s">
-        <v>42</v>
-      </c>
-      <c r="D37" s="80" t="s">
-        <v>144</v>
-      </c>
+      <c r="B37" s="118" t="s">
+        <v>161</v>
+      </c>
+      <c r="C37" s="109" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="80"/>
       <c r="E37" s="45" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F37" s="45" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G37" s="93" t="s">
         <v>196</v>
@@ -9346,13 +9379,13 @@
       <c r="I37" s="48"/>
       <c r="J37" s="48"/>
       <c r="K37" s="48">
-        <v>45769</v>
+        <v>45737</v>
       </c>
       <c r="L37" s="48">
-        <v>45772</v>
-      </c>
-      <c r="M37" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L37, H37&lt;1), -1, IF(H37=1, 1, 0))</f>
+        <v>45744</v>
+      </c>
+      <c r="M37" s="115">
+        <f t="shared" ca="1" si="70"/>
         <v>0</v>
       </c>
       <c r="N37" s="3"/>
@@ -9497,41 +9530,39 @@
       <c r="EW37" s="38"/>
       <c r="EX37" s="38"/>
     </row>
-    <row r="38" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A38" s="12"/>
-      <c r="B38" s="92" t="s">
-        <v>146</v>
-      </c>
-      <c r="C38" s="140" t="s">
-        <v>43</v>
-      </c>
-      <c r="D38" s="80"/>
+      <c r="B38" s="122" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" s="109" t="s">
+        <v>182</v>
+      </c>
+      <c r="D38" s="80" t="s">
+        <v>184</v>
+      </c>
       <c r="E38" s="45" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="F38" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="G38" s="93" t="s">
+        <v>87</v>
+      </c>
+      <c r="G38" s="134" t="s">
         <v>196</v>
       </c>
       <c r="H38" s="47">
-        <v>0.8</v>
-      </c>
-      <c r="I38" s="48">
-        <v>45705</v>
-      </c>
-      <c r="J38" s="48">
-        <v>45709</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I38" s="48"/>
+      <c r="J38" s="48"/>
       <c r="K38" s="48">
-        <v>45719</v>
+        <v>45747</v>
       </c>
       <c r="L38" s="48">
-        <v>45721</v>
-      </c>
-      <c r="M38" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L38, H38&lt;1), -1, IF(H38=1, 1, 0))</f>
+        <v>45758</v>
+      </c>
+      <c r="M38" s="115">
+        <f t="shared" ca="1" si="70"/>
         <v>0</v>
       </c>
       <c r="N38" s="3"/>
@@ -9676,39 +9707,37 @@
       <c r="EW38" s="38"/>
       <c r="EX38" s="38"/>
     </row>
-    <row r="39" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A39" s="12"/>
-      <c r="B39" s="96" t="s">
-        <v>147</v>
-      </c>
-      <c r="C39" s="140" t="s">
-        <v>44</v>
-      </c>
-      <c r="D39" s="80" t="s">
-        <v>131</v>
-      </c>
-      <c r="E39" s="45" t="s">
+      <c r="B39" s="151" t="s">
+        <v>129</v>
+      </c>
+      <c r="C39" s="127" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" s="128"/>
+      <c r="E39" s="121" t="s">
         <v>70</v>
       </c>
-      <c r="F39" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="G39" s="93" t="s">
+      <c r="F39" s="121" t="s">
+        <v>95</v>
+      </c>
+      <c r="G39" s="136" t="s">
         <v>196</v>
       </c>
-      <c r="H39" s="47">
+      <c r="H39" s="140">
         <v>0</v>
       </c>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
-      <c r="K39" s="48">
-        <v>45722</v>
-      </c>
-      <c r="L39" s="48">
-        <v>45723</v>
-      </c>
-      <c r="M39" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L39, H39&lt;1), -1, IF(H39=1, 1, 0))</f>
+      <c r="I39" s="144"/>
+      <c r="J39" s="144"/>
+      <c r="K39" s="144">
+        <v>45761</v>
+      </c>
+      <c r="L39" s="144">
+        <v>45765</v>
+      </c>
+      <c r="M39" s="115">
+        <f t="shared" ca="1" si="70"/>
         <v>0</v>
       </c>
       <c r="N39" s="3"/>
@@ -9853,22 +9882,22 @@
       <c r="EW39" s="38"/>
       <c r="EX39" s="38"/>
     </row>
-    <row r="40" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A40" s="12"/>
-      <c r="B40" s="92" t="s">
-        <v>148</v>
-      </c>
-      <c r="C40" s="140" t="s">
-        <v>51</v>
-      </c>
-      <c r="D40" s="80"/>
+      <c r="B40" s="123" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" s="109" t="s">
+        <v>187</v>
+      </c>
+      <c r="D40" s="94"/>
       <c r="E40" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="F40" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="G40" s="93" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" s="131" t="s">
+        <v>103</v>
+      </c>
+      <c r="G40" s="134" t="s">
         <v>196</v>
       </c>
       <c r="H40" s="47">
@@ -9877,13 +9906,13 @@
       <c r="I40" s="48"/>
       <c r="J40" s="48"/>
       <c r="K40" s="48">
-        <v>45712</v>
+        <v>45768</v>
       </c>
       <c r="L40" s="48">
-        <v>45713</v>
-      </c>
-      <c r="M40" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L40, H40&lt;1), -1, IF(H40=1, 1, 0))</f>
+        <v>45772</v>
+      </c>
+      <c r="M40" s="115">
+        <f t="shared" ca="1" si="70"/>
         <v>0</v>
       </c>
       <c r="N40" s="3"/>
@@ -10028,42 +10057,42 @@
       <c r="EW40" s="38"/>
       <c r="EX40" s="38"/>
     </row>
-    <row r="41" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A41" s="12"/>
-      <c r="B41" s="96" t="s">
-        <v>149</v>
-      </c>
-      <c r="C41" s="140" t="s">
-        <v>53</v>
-      </c>
-      <c r="D41" s="80"/>
+      <c r="B41" s="118" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="109" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="94"/>
       <c r="E41" s="45" t="s">
         <v>70</v>
       </c>
       <c r="F41" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="G41" s="93" t="s">
+        <v>103</v>
+      </c>
+      <c r="G41" s="134" t="s">
         <v>196</v>
       </c>
       <c r="H41" s="47">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="I41" s="48"/>
       <c r="J41" s="48"/>
       <c r="K41" s="48">
-        <v>45712</v>
+        <v>45775</v>
       </c>
       <c r="L41" s="48">
-        <v>45713</v>
-      </c>
-      <c r="M41" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L41, H41&lt;1), -1, IF(H41=1, 1, 0))</f>
+        <v>45777</v>
+      </c>
+      <c r="M41" s="115">
+        <f t="shared" ca="1" si="70"/>
         <v>0</v>
       </c>
       <c r="N41" s="3">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O41" s="38"/>
       <c r="P41" s="38"/>
@@ -10206,13 +10235,13 @@
       <c r="EW41" s="38"/>
       <c r="EX41" s="38"/>
     </row>
-    <row r="42" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A42" s="12"/>
-      <c r="B42" s="101"/>
-      <c r="C42" s="139" t="s">
+      <c r="B42" s="95"/>
+      <c r="C42" s="108" t="s">
         <v>192</v>
       </c>
-      <c r="D42" s="101"/>
+      <c r="D42" s="95"/>
       <c r="E42" s="45"/>
       <c r="F42" s="45"/>
       <c r="G42" s="46"/>
@@ -10221,7 +10250,7 @@
       <c r="J42" s="48"/>
       <c r="K42" s="48"/>
       <c r="L42" s="48"/>
-      <c r="M42" s="148"/>
+      <c r="M42" s="115"/>
       <c r="N42" s="3" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
@@ -10367,13 +10396,13 @@
       <c r="EW42" s="38"/>
       <c r="EX42" s="38"/>
     </row>
-    <row r="43" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A43" s="12"/>
       <c r="B43" s="80" t="s">
-        <v>150</v>
-      </c>
-      <c r="C43" s="140" t="s">
-        <v>46</v>
+        <v>152</v>
+      </c>
+      <c r="C43" s="109" t="s">
+        <v>47</v>
       </c>
       <c r="D43" s="80"/>
       <c r="E43" s="45" t="s">
@@ -10391,18 +10420,18 @@
       <c r="I43" s="48"/>
       <c r="J43" s="48"/>
       <c r="K43" s="48">
-        <v>45710</v>
+        <v>45777</v>
       </c>
       <c r="L43" s="48">
-        <v>45711</v>
-      </c>
-      <c r="M43" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L43, H43&lt;1), -1, IF(H43=1, 1, 0))</f>
+        <v>45777</v>
+      </c>
+      <c r="M43" s="115">
+        <f t="shared" ref="M43:M51" ca="1" si="71">IF(AND(TODAY()&gt;L43, H43&lt;1), -1, IF(H43=1, 1, 0))</f>
         <v>1</v>
       </c>
       <c r="N43" s="3">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O43" s="38"/>
       <c r="P43" s="38"/>
@@ -10545,15 +10574,15 @@
       <c r="EW43" s="38"/>
       <c r="EX43" s="38"/>
     </row>
-    <row r="44" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A44" s="12"/>
-      <c r="B44" s="100" t="s">
-        <v>151</v>
-      </c>
-      <c r="C44" s="140" t="s">
-        <v>187</v>
-      </c>
-      <c r="D44" s="100"/>
+      <c r="B44" s="94" t="s">
+        <v>153</v>
+      </c>
+      <c r="C44" s="109" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="80"/>
       <c r="E44" s="45" t="s">
         <v>33</v>
       </c>
@@ -10564,19 +10593,19 @@
         <v>196</v>
       </c>
       <c r="H44" s="47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" s="48"/>
       <c r="J44" s="48"/>
       <c r="K44" s="48">
-        <v>45747</v>
+        <v>45777</v>
       </c>
       <c r="L44" s="48">
-        <v>45751</v>
-      </c>
-      <c r="M44" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L44, H44&lt;1), -1, IF(H44=1, 1, 0))</f>
-        <v>0</v>
+        <v>45777</v>
+      </c>
+      <c r="M44" s="115">
+        <f t="shared" ca="1" si="71"/>
+        <v>1</v>
       </c>
       <c r="N44" s="3"/>
       <c r="O44" s="38"/>
@@ -10720,42 +10749,42 @@
       <c r="EW44" s="38"/>
       <c r="EX44" s="38"/>
     </row>
-    <row r="45" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A45" s="12"/>
       <c r="B45" s="80" t="s">
-        <v>152</v>
-      </c>
-      <c r="C45" s="140" t="s">
-        <v>47</v>
+        <v>156</v>
+      </c>
+      <c r="C45" s="109" t="s">
+        <v>188</v>
       </c>
       <c r="D45" s="80"/>
       <c r="E45" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="F45" s="81" t="s">
-        <v>103</v>
+        <v>70</v>
+      </c>
+      <c r="F45" s="130" t="s">
+        <v>87</v>
       </c>
       <c r="G45" s="46" t="s">
         <v>196</v>
       </c>
       <c r="H45" s="47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" s="48"/>
       <c r="J45" s="48"/>
       <c r="K45" s="48">
-        <v>45762</v>
+        <v>45777</v>
       </c>
       <c r="L45" s="48">
-        <v>45763</v>
-      </c>
-      <c r="M45" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L45, H45&lt;1), -1, IF(H45=1, 1, 0))</f>
-        <v>1</v>
+        <v>45779</v>
+      </c>
+      <c r="M45" s="115">
+        <f t="shared" ca="1" si="71"/>
+        <v>0</v>
       </c>
       <c r="N45" s="3">
-        <f t="shared" ref="N45:N51" si="69">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v>2</v>
+        <f t="shared" ref="N45:N51" si="72">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v>3</v>
       </c>
       <c r="O45" s="38"/>
       <c r="P45" s="38"/>
@@ -10898,42 +10927,42 @@
       <c r="EW45" s="38"/>
       <c r="EX45" s="38"/>
     </row>
-    <row r="46" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A46" s="12"/>
-      <c r="B46" s="100" t="s">
-        <v>153</v>
-      </c>
-      <c r="C46" s="140" t="s">
-        <v>48</v>
+      <c r="B46" s="94" t="s">
+        <v>190</v>
+      </c>
+      <c r="C46" s="109" t="s">
+        <v>191</v>
       </c>
       <c r="D46" s="80"/>
       <c r="E46" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="F46" s="81" t="s">
+        <v>70</v>
+      </c>
+      <c r="F46" s="130" t="s">
         <v>103</v>
       </c>
       <c r="G46" s="46" t="s">
         <v>196</v>
       </c>
       <c r="H46" s="47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I46" s="48"/>
       <c r="J46" s="48"/>
       <c r="K46" s="48">
-        <v>45761</v>
+        <v>45777</v>
       </c>
       <c r="L46" s="48">
-        <v>45761</v>
-      </c>
-      <c r="M46" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L46, H46&lt;1), -1, IF(H46=1, 1, 0))</f>
-        <v>1</v>
+        <v>45780</v>
+      </c>
+      <c r="M46" s="115">
+        <f t="shared" ca="1" si="71"/>
+        <v>0</v>
       </c>
       <c r="N46" s="3">
-        <f t="shared" si="69"/>
-        <v>1</v>
+        <f t="shared" si="72"/>
+        <v>4</v>
       </c>
       <c r="O46" s="38"/>
       <c r="P46" s="38"/>
@@ -11076,15 +11105,15 @@
       <c r="EW46" s="38"/>
       <c r="EX46" s="38"/>
     </row>
-    <row r="47" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A47" s="12"/>
       <c r="B47" s="80" t="s">
         <v>154</v>
       </c>
-      <c r="C47" s="140" t="s">
+      <c r="C47" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="100"/>
+      <c r="D47" s="94"/>
       <c r="E47" s="45" t="s">
         <v>70</v>
       </c>
@@ -11100,18 +11129,18 @@
       <c r="I47" s="48"/>
       <c r="J47" s="48"/>
       <c r="K47" s="48">
-        <v>45765</v>
+        <v>45779</v>
       </c>
       <c r="L47" s="48">
-        <v>45768</v>
-      </c>
-      <c r="M47" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L47, H47&lt;1), -1, IF(H47=1, 1, 0))</f>
+        <v>45789</v>
+      </c>
+      <c r="M47" s="115">
+        <f t="shared" ca="1" si="71"/>
         <v>0</v>
       </c>
       <c r="N47" s="3">
-        <f t="shared" si="69"/>
-        <v>4</v>
+        <f t="shared" si="72"/>
+        <v>11</v>
       </c>
       <c r="O47" s="38"/>
       <c r="P47" s="38"/>
@@ -11254,42 +11283,46 @@
       <c r="EW47" s="38"/>
       <c r="EX47" s="38"/>
     </row>
-    <row r="48" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A48" s="12"/>
-      <c r="B48" s="100" t="s">
-        <v>155</v>
-      </c>
-      <c r="C48" s="140" t="s">
-        <v>50</v>
-      </c>
-      <c r="D48" s="100"/>
+      <c r="B48" s="119" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" s="109" t="s">
+        <v>43</v>
+      </c>
+      <c r="D48" s="80"/>
       <c r="E48" s="45" t="s">
         <v>70</v>
       </c>
       <c r="F48" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="G48" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="G48" s="135" t="s">
         <v>196</v>
       </c>
       <c r="H48" s="47">
         <v>0.8</v>
       </c>
-      <c r="I48" s="48"/>
-      <c r="J48" s="48"/>
+      <c r="I48" s="48">
+        <v>45705</v>
+      </c>
+      <c r="J48" s="48">
+        <v>45709</v>
+      </c>
       <c r="K48" s="48">
-        <v>45754</v>
+        <v>45786</v>
       </c>
       <c r="L48" s="48">
-        <v>45756</v>
-      </c>
-      <c r="M48" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L48, H48&lt;1), -1, IF(H48=1, 1, 0))</f>
+        <v>45790</v>
+      </c>
+      <c r="M48" s="115">
+        <f t="shared" ca="1" si="71"/>
         <v>0</v>
       </c>
       <c r="N48" s="3">
-        <f t="shared" si="69"/>
-        <v>3</v>
+        <f t="shared" si="72"/>
+        <v>5</v>
       </c>
       <c r="O48" s="38"/>
       <c r="P48" s="38"/>
@@ -11432,22 +11465,24 @@
       <c r="EW48" s="38"/>
       <c r="EX48" s="38"/>
     </row>
-    <row r="49" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A49" s="12"/>
-      <c r="B49" s="80" t="s">
-        <v>156</v>
-      </c>
-      <c r="C49" s="140" t="s">
-        <v>188</v>
-      </c>
-      <c r="D49" s="80"/>
+      <c r="B49" s="119" t="s">
+        <v>147</v>
+      </c>
+      <c r="C49" s="109" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="80" t="s">
+        <v>131</v>
+      </c>
       <c r="E49" s="45" t="s">
         <v>70</v>
       </c>
       <c r="F49" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="G49" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="G49" s="135" t="s">
         <v>196</v>
       </c>
       <c r="H49" s="47">
@@ -11456,18 +11491,18 @@
       <c r="I49" s="48"/>
       <c r="J49" s="48"/>
       <c r="K49" s="48">
-        <v>45757</v>
+        <v>45786</v>
       </c>
       <c r="L49" s="48">
-        <v>45758</v>
-      </c>
-      <c r="M49" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L49, H49&lt;1), -1, IF(H49=1, 1, 0))</f>
+        <v>45790</v>
+      </c>
+      <c r="M49" s="115">
+        <f t="shared" ca="1" si="71"/>
         <v>0</v>
       </c>
       <c r="N49" s="3">
-        <f t="shared" si="69"/>
-        <v>2</v>
+        <f t="shared" si="72"/>
+        <v>5</v>
       </c>
       <c r="O49" s="38"/>
       <c r="P49" s="38"/>
@@ -11610,20 +11645,20 @@
       <c r="EW49" s="38"/>
       <c r="EX49" s="38"/>
     </row>
-    <row r="50" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A50" s="12"/>
-      <c r="B50" s="100" t="s">
-        <v>157</v>
-      </c>
-      <c r="C50" s="140" t="s">
-        <v>189</v>
+      <c r="B50" s="80" t="s">
+        <v>141</v>
+      </c>
+      <c r="C50" s="109" t="s">
+        <v>106</v>
       </c>
       <c r="D50" s="80"/>
       <c r="E50" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="F50" s="45" t="s">
-        <v>87</v>
+      <c r="F50" s="131" t="s">
+        <v>103</v>
       </c>
       <c r="G50" s="46" t="s">
         <v>196</v>
@@ -11634,13 +11669,13 @@
       <c r="I50" s="48"/>
       <c r="J50" s="48"/>
       <c r="K50" s="48">
-        <v>45764</v>
+        <v>45787</v>
       </c>
       <c r="L50" s="48">
-        <v>45764</v>
-      </c>
-      <c r="M50" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L50, H50&lt;1), -1, IF(H50=1, 1, 0))</f>
+        <v>45789</v>
+      </c>
+      <c r="M50" s="115">
+        <f t="shared" ca="1" si="71"/>
         <v>0</v>
       </c>
       <c r="N50" s="3"/>
@@ -11785,20 +11820,20 @@
       <c r="EW50" s="38"/>
       <c r="EX50" s="38"/>
     </row>
-    <row r="51" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A51" s="12"/>
-      <c r="B51" s="100" t="s">
-        <v>190</v>
-      </c>
-      <c r="C51" s="140" t="s">
-        <v>191</v>
+      <c r="B51" s="94" t="s">
+        <v>157</v>
+      </c>
+      <c r="C51" s="109" t="s">
+        <v>189</v>
       </c>
       <c r="D51" s="80"/>
       <c r="E51" s="45" t="s">
         <v>70</v>
       </c>
       <c r="F51" s="45" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="G51" s="46" t="s">
         <v>196</v>
@@ -11809,18 +11844,18 @@
       <c r="I51" s="48"/>
       <c r="J51" s="48"/>
       <c r="K51" s="48">
-        <v>45764</v>
+        <v>45789</v>
       </c>
       <c r="L51" s="48">
-        <v>45764</v>
-      </c>
-      <c r="M51" s="148">
-        <f ca="1">IF(AND(TODAY()&gt;L51, H51&lt;1), -1, IF(H51=1, 1, 0))</f>
+        <v>45792</v>
+      </c>
+      <c r="M51" s="115">
+        <f t="shared" ca="1" si="71"/>
         <v>0</v>
       </c>
       <c r="N51" s="3">
-        <f t="shared" si="69"/>
-        <v>1</v>
+        <f t="shared" si="72"/>
+        <v>4</v>
       </c>
       <c r="O51" s="38"/>
       <c r="P51" s="38"/>
@@ -11963,13 +11998,13 @@
       <c r="EW51" s="38"/>
       <c r="EX51" s="38"/>
     </row>
-    <row r="52" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A52" s="12"/>
       <c r="B52" s="80"/>
-      <c r="C52" s="139" t="s">
+      <c r="C52" s="108" t="s">
         <v>102</v>
       </c>
-      <c r="D52" s="101"/>
+      <c r="D52" s="95"/>
       <c r="E52" s="45"/>
       <c r="F52" s="45"/>
       <c r="G52" s="46"/>
@@ -11978,7 +12013,7 @@
       <c r="J52" s="48"/>
       <c r="K52" s="48"/>
       <c r="L52" s="48"/>
-      <c r="M52" s="148"/>
+      <c r="M52" s="115"/>
       <c r="N52" s="3"/>
       <c r="O52" s="38"/>
       <c r="P52" s="38"/>
@@ -12121,12 +12156,12 @@
       <c r="EW52" s="38"/>
       <c r="EX52" s="38"/>
     </row>
-    <row r="53" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A53" s="12"/>
       <c r="B53" s="80" t="s">
         <v>168</v>
       </c>
-      <c r="C53" s="140" t="s">
+      <c r="C53" s="109" t="s">
         <v>91</v>
       </c>
       <c r="D53" s="80" t="s">
@@ -12152,7 +12187,7 @@
       <c r="L53" s="48">
         <v>45809</v>
       </c>
-      <c r="M53" s="148">
+      <c r="M53" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L53, H53&lt;1), -1, IF(H53=1, 1, 0))</f>
         <v>0</v>
       </c>
@@ -12298,12 +12333,12 @@
       <c r="EW53" s="38"/>
       <c r="EX53" s="38"/>
     </row>
-    <row r="54" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A54" s="12"/>
-      <c r="B54" s="100" t="s">
+      <c r="B54" s="94" t="s">
         <v>173</v>
       </c>
-      <c r="C54" s="140" t="s">
+      <c r="C54" s="109" t="s">
         <v>92</v>
       </c>
       <c r="D54" s="80" t="s">
@@ -12329,7 +12364,7 @@
       <c r="L54" s="48">
         <v>45809</v>
       </c>
-      <c r="M54" s="148">
+      <c r="M54" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L54, H54&lt;1), -1, IF(H54=1, 1, 0))</f>
         <v>0</v>
       </c>
@@ -12475,12 +12510,12 @@
       <c r="EW54" s="38"/>
       <c r="EX54" s="38"/>
     </row>
-    <row r="55" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A55" s="12"/>
       <c r="B55" s="80" t="s">
         <v>169</v>
       </c>
-      <c r="C55" s="140" t="s">
+      <c r="C55" s="109" t="s">
         <v>93</v>
       </c>
       <c r="D55" s="80" t="s">
@@ -12506,7 +12541,7 @@
       <c r="L55" s="48">
         <v>45809</v>
       </c>
-      <c r="M55" s="148">
+      <c r="M55" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L55, H55&lt;1), -1, IF(H55=1, 1, 0))</f>
         <v>0</v>
       </c>
@@ -12652,13 +12687,13 @@
       <c r="EW55" s="38"/>
       <c r="EX55" s="38"/>
     </row>
-    <row r="56" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A56" s="12"/>
-      <c r="B56" s="100"/>
-      <c r="C56" s="139" t="s">
+      <c r="B56" s="94"/>
+      <c r="C56" s="108" t="s">
         <v>113</v>
       </c>
-      <c r="D56" s="101"/>
+      <c r="D56" s="95"/>
       <c r="E56" s="45"/>
       <c r="F56" s="45"/>
       <c r="G56" s="46"/>
@@ -12667,7 +12702,7 @@
       <c r="J56" s="48"/>
       <c r="K56" s="48"/>
       <c r="L56" s="48"/>
-      <c r="M56" s="148"/>
+      <c r="M56" s="115"/>
       <c r="N56" s="3"/>
       <c r="O56" s="38"/>
       <c r="P56" s="38"/>
@@ -12810,38 +12845,38 @@
       <c r="EW56" s="38"/>
       <c r="EX56" s="38"/>
     </row>
-    <row r="57" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A57" s="12"/>
-      <c r="B57" s="100" t="s">
-        <v>158</v>
-      </c>
-      <c r="C57" s="141" t="s">
-        <v>112</v>
-      </c>
-      <c r="D57" s="92" t="s">
-        <v>130</v>
-      </c>
-      <c r="E57" s="81" t="s">
-        <v>63</v>
-      </c>
-      <c r="F57" s="81" t="s">
-        <v>103</v>
+      <c r="B57" s="119" t="s">
+        <v>145</v>
+      </c>
+      <c r="C57" s="124" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" s="122" t="s">
+        <v>144</v>
+      </c>
+      <c r="E57" s="130" t="s">
+        <v>69</v>
+      </c>
+      <c r="F57" s="130" t="s">
+        <v>96</v>
       </c>
       <c r="G57" s="93" t="s">
         <v>196</v>
       </c>
-      <c r="H57" s="94">
+      <c r="H57" s="137">
         <v>0</v>
       </c>
-      <c r="I57" s="95"/>
-      <c r="J57" s="95"/>
-      <c r="K57" s="48" t="s">
-        <v>202</v>
-      </c>
-      <c r="L57" s="48" t="s">
-        <v>203</v>
-      </c>
-      <c r="M57" s="148">
+      <c r="I57" s="141"/>
+      <c r="J57" s="141"/>
+      <c r="K57" s="48">
+        <v>45796</v>
+      </c>
+      <c r="L57" s="48">
+        <v>45800</v>
+      </c>
+      <c r="M57" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L57, H57&lt;1), -1, IF(H57=1, 1, 0))</f>
         <v>0</v>
       </c>
@@ -12987,22 +13022,24 @@
       <c r="EW57" s="38"/>
       <c r="EX57" s="38"/>
     </row>
-    <row r="58" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A58" s="12"/>
       <c r="B58" s="80" t="s">
-        <v>159</v>
-      </c>
-      <c r="C58" s="140" t="s">
-        <v>65</v>
-      </c>
-      <c r="D58" s="80"/>
+        <v>164</v>
+      </c>
+      <c r="C58" s="109" t="s">
+        <v>195</v>
+      </c>
+      <c r="D58" s="80" t="s">
+        <v>184</v>
+      </c>
       <c r="E58" s="45" t="s">
-        <v>70</v>
+        <v>183</v>
       </c>
       <c r="F58" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="G58" s="93" t="s">
+      <c r="G58" s="134" t="s">
         <v>196</v>
       </c>
       <c r="H58" s="47">
@@ -13011,12 +13048,12 @@
       <c r="I58" s="48"/>
       <c r="J58" s="48"/>
       <c r="K58" s="48">
-        <v>45714</v>
+        <v>45803</v>
       </c>
       <c r="L58" s="48">
-        <v>45716</v>
-      </c>
-      <c r="M58" s="148">
+        <v>45807</v>
+      </c>
+      <c r="M58" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L58, H58&lt;1), -1, IF(H58=1, 1, 0))</f>
         <v>0</v>
       </c>
@@ -13162,36 +13199,36 @@
       <c r="EW58" s="38"/>
       <c r="EX58" s="38"/>
     </row>
-    <row r="59" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A59" s="12"/>
-      <c r="B59" s="100" t="s">
-        <v>160</v>
-      </c>
-      <c r="C59" s="140" t="s">
-        <v>186</v>
-      </c>
-      <c r="D59" s="80"/>
-      <c r="E59" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="F59" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="G59" s="93" t="s">
+      <c r="B59" s="121" t="s">
+        <v>130</v>
+      </c>
+      <c r="C59" s="127" t="s">
+        <v>104</v>
+      </c>
+      <c r="D59" s="128"/>
+      <c r="E59" s="121" t="s">
+        <v>33</v>
+      </c>
+      <c r="F59" s="121" t="s">
+        <v>95</v>
+      </c>
+      <c r="G59" s="136" t="s">
         <v>196</v>
       </c>
-      <c r="H59" s="47">
+      <c r="H59" s="140">
         <v>0</v>
       </c>
-      <c r="I59" s="48"/>
-      <c r="J59" s="48"/>
-      <c r="K59" s="48">
-        <v>45714</v>
-      </c>
-      <c r="L59" s="48">
-        <v>45716</v>
-      </c>
-      <c r="M59" s="148">
+      <c r="I59" s="144"/>
+      <c r="J59" s="144"/>
+      <c r="K59" s="144">
+        <v>45810</v>
+      </c>
+      <c r="L59" s="144">
+        <v>45812</v>
+      </c>
+      <c r="M59" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L59, H59&lt;1), -1, IF(H59=1, 1, 0))</f>
         <v>0</v>
       </c>
@@ -13337,22 +13374,24 @@
       <c r="EW59" s="38"/>
       <c r="EX59" s="38"/>
     </row>
-    <row r="60" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A60" s="12"/>
-      <c r="B60" s="100" t="s">
-        <v>161</v>
-      </c>
-      <c r="C60" s="140" t="s">
-        <v>66</v>
-      </c>
-      <c r="D60" s="80"/>
+      <c r="B60" s="80" t="s">
+        <v>138</v>
+      </c>
+      <c r="C60" s="109" t="s">
+        <v>111</v>
+      </c>
+      <c r="D60" s="80" t="s">
+        <v>130</v>
+      </c>
       <c r="E60" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="F60" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="G60" s="93" t="s">
+        <v>63</v>
+      </c>
+      <c r="F60" s="131" t="s">
+        <v>103</v>
+      </c>
+      <c r="G60" s="134" t="s">
         <v>196</v>
       </c>
       <c r="H60" s="47">
@@ -13361,18 +13400,18 @@
       <c r="I60" s="48"/>
       <c r="J60" s="48"/>
       <c r="K60" s="48">
-        <v>45714</v>
+        <v>45813</v>
       </c>
       <c r="L60" s="48">
-        <v>45716</v>
-      </c>
-      <c r="M60" s="148">
+        <v>45825</v>
+      </c>
+      <c r="M60" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L60, H60&lt;1), -1, IF(H60=1, 1, 0))</f>
         <v>0</v>
       </c>
       <c r="N60" s="3">
-        <f t="shared" ref="N60:N69" si="70">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v>3</v>
+        <f t="shared" ref="N60:N69" si="73">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v>13</v>
       </c>
       <c r="O60" s="38"/>
       <c r="P60" s="38"/>
@@ -13515,13 +13554,13 @@
       <c r="EW60" s="38"/>
       <c r="EX60" s="38"/>
     </row>
-    <row r="61" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A61" s="12"/>
       <c r="B61" s="80"/>
-      <c r="C61" s="139" t="s">
+      <c r="C61" s="108" t="s">
         <v>101</v>
       </c>
-      <c r="D61" s="101"/>
+      <c r="D61" s="95"/>
       <c r="E61" s="45"/>
       <c r="F61" s="45"/>
       <c r="G61" s="46"/>
@@ -13530,9 +13569,9 @@
       <c r="J61" s="48"/>
       <c r="K61" s="48"/>
       <c r="L61" s="48"/>
-      <c r="M61" s="148"/>
+      <c r="M61" s="115"/>
       <c r="N61" s="3" t="str">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v/>
       </c>
       <c r="O61" s="38"/>
@@ -13676,44 +13715,44 @@
       <c r="EW61" s="38"/>
       <c r="EX61" s="38"/>
     </row>
-    <row r="62" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A62" s="12"/>
-      <c r="B62" s="100" t="s">
-        <v>162</v>
-      </c>
-      <c r="C62" s="140" t="s">
-        <v>67</v>
-      </c>
-      <c r="D62" s="80" t="s">
-        <v>184</v>
-      </c>
-      <c r="E62" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="F62" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="G62" s="46" t="s">
+      <c r="B62" s="94" t="s">
+        <v>158</v>
+      </c>
+      <c r="C62" s="125" t="s">
+        <v>112</v>
+      </c>
+      <c r="D62" s="119" t="s">
+        <v>130</v>
+      </c>
+      <c r="E62" s="131" t="s">
+        <v>63</v>
+      </c>
+      <c r="F62" s="131" t="s">
+        <v>103</v>
+      </c>
+      <c r="G62" s="135" t="s">
         <v>196</v>
       </c>
-      <c r="H62" s="47">
+      <c r="H62" s="138">
         <v>0</v>
       </c>
-      <c r="I62" s="48"/>
-      <c r="J62" s="48"/>
+      <c r="I62" s="142"/>
+      <c r="J62" s="142"/>
       <c r="K62" s="48">
-        <v>45705</v>
+        <v>45813</v>
       </c>
       <c r="L62" s="48">
-        <v>45711</v>
-      </c>
-      <c r="M62" s="148">
+        <v>45825</v>
+      </c>
+      <c r="M62" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L62, H62&lt;1), -1, IF(H62=1, 1, 0))</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N62" s="3">
-        <f t="shared" si="70"/>
-        <v>7</v>
+        <f t="shared" si="73"/>
+        <v>13</v>
       </c>
       <c r="O62" s="38"/>
       <c r="P62" s="38"/>
@@ -13856,44 +13895,44 @@
       <c r="EW62" s="38"/>
       <c r="EX62" s="38"/>
     </row>
-    <row r="63" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A63" s="12"/>
-      <c r="B63" s="80" t="s">
-        <v>163</v>
-      </c>
-      <c r="C63" s="140" t="s">
-        <v>182</v>
-      </c>
-      <c r="D63" s="80" t="s">
-        <v>184</v>
-      </c>
-      <c r="E63" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="F63" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="G63" s="46" t="s">
+      <c r="B63" s="119" t="s">
+        <v>142</v>
+      </c>
+      <c r="C63" s="125" t="s">
+        <v>179</v>
+      </c>
+      <c r="D63" s="119" t="s">
+        <v>181</v>
+      </c>
+      <c r="E63" s="131" t="s">
+        <v>74</v>
+      </c>
+      <c r="F63" s="131" t="s">
+        <v>96</v>
+      </c>
+      <c r="G63" s="135" t="s">
         <v>196</v>
       </c>
-      <c r="H63" s="47">
+      <c r="H63" s="138">
         <v>0</v>
       </c>
-      <c r="I63" s="48"/>
-      <c r="J63" s="48"/>
-      <c r="K63" s="48">
-        <v>45726</v>
-      </c>
-      <c r="L63" s="48">
-        <v>45737</v>
-      </c>
-      <c r="M63" s="148">
+      <c r="I63" s="142"/>
+      <c r="J63" s="142"/>
+      <c r="K63" s="142">
+        <v>45826</v>
+      </c>
+      <c r="L63" s="142">
+        <v>45828</v>
+      </c>
+      <c r="M63" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L63, H63&lt;1), -1, IF(H63=1, 1, 0))</f>
         <v>0</v>
       </c>
       <c r="N63" s="3">
-        <f t="shared" si="70"/>
-        <v>12</v>
+        <f t="shared" si="73"/>
+        <v>3</v>
       </c>
       <c r="O63" s="38"/>
       <c r="P63" s="38"/>
@@ -14036,44 +14075,44 @@
       <c r="EW63" s="38"/>
       <c r="EX63" s="38"/>
     </row>
-    <row r="64" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A64" s="12"/>
-      <c r="B64" s="80" t="s">
-        <v>164</v>
-      </c>
-      <c r="C64" s="140" t="s">
-        <v>195</v>
-      </c>
-      <c r="D64" s="80" t="s">
-        <v>184</v>
-      </c>
-      <c r="E64" s="45" t="s">
-        <v>183</v>
-      </c>
-      <c r="F64" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="G64" s="46" t="s">
+      <c r="B64" s="119" t="s">
+        <v>143</v>
+      </c>
+      <c r="C64" s="125" t="s">
+        <v>180</v>
+      </c>
+      <c r="D64" s="119" t="s">
+        <v>181</v>
+      </c>
+      <c r="E64" s="131" t="s">
+        <v>72</v>
+      </c>
+      <c r="F64" s="131" t="s">
+        <v>96</v>
+      </c>
+      <c r="G64" s="135" t="s">
         <v>196</v>
       </c>
-      <c r="H64" s="47">
+      <c r="H64" s="138">
         <v>0</v>
       </c>
-      <c r="I64" s="48"/>
-      <c r="J64" s="48"/>
-      <c r="K64" s="48">
-        <v>45775</v>
-      </c>
-      <c r="L64" s="48">
-        <v>45777</v>
-      </c>
-      <c r="M64" s="148">
+      <c r="I64" s="142"/>
+      <c r="J64" s="142"/>
+      <c r="K64" s="142">
+        <v>45831</v>
+      </c>
+      <c r="L64" s="142">
+        <v>45838</v>
+      </c>
+      <c r="M64" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L64, H64&lt;1), -1, IF(H64=1, 1, 0))</f>
         <v>0</v>
       </c>
       <c r="N64" s="3">
-        <f t="shared" si="70"/>
-        <v>3</v>
+        <f t="shared" si="73"/>
+        <v>8</v>
       </c>
       <c r="O64" s="38"/>
       <c r="P64" s="38"/>
@@ -14216,13 +14255,13 @@
       <c r="EW64" s="38"/>
       <c r="EX64" s="38"/>
     </row>
-    <row r="65" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A65" s="12"/>
-      <c r="B65" s="101"/>
-      <c r="C65" s="139" t="s">
+      <c r="B65" s="95"/>
+      <c r="C65" s="108" t="s">
         <v>100</v>
       </c>
-      <c r="D65" s="101"/>
+      <c r="D65" s="95"/>
       <c r="E65" s="45"/>
       <c r="F65" s="45"/>
       <c r="G65" s="46"/>
@@ -14231,9 +14270,9 @@
       <c r="J65" s="48"/>
       <c r="K65" s="48"/>
       <c r="L65" s="48"/>
-      <c r="M65" s="148"/>
+      <c r="M65" s="115"/>
       <c r="N65" s="3" t="str">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v/>
       </c>
       <c r="O65" s="38"/>
@@ -14377,12 +14416,12 @@
       <c r="EW65" s="38"/>
       <c r="EX65" s="38"/>
     </row>
-    <row r="66" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A66" s="12"/>
       <c r="B66" s="80" t="s">
         <v>165</v>
       </c>
-      <c r="C66" s="140" t="s">
+      <c r="C66" s="109" t="s">
         <v>185</v>
       </c>
       <c r="D66" s="80"/>
@@ -14410,12 +14449,12 @@
       <c r="L66" s="48">
         <v>45723</v>
       </c>
-      <c r="M66" s="148">
+      <c r="M66" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L66, H66&lt;1), -1, IF(H66=1, 1, 0))</f>
         <v>0</v>
       </c>
       <c r="N66" s="3">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v>7</v>
       </c>
       <c r="O66" s="38"/>
@@ -14559,12 +14598,12 @@
       <c r="EW66" s="38"/>
       <c r="EX66" s="38"/>
     </row>
-    <row r="67" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A67" s="12"/>
       <c r="B67" s="80" t="s">
         <v>166</v>
       </c>
-      <c r="C67" s="140" t="s">
+      <c r="C67" s="109" t="s">
         <v>57</v>
       </c>
       <c r="D67" s="80" t="s">
@@ -14594,12 +14633,12 @@
       <c r="L67" s="48">
         <v>45730</v>
       </c>
-      <c r="M67" s="148">
+      <c r="M67" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L67, H67&lt;1), -1, IF(H67=1, 1, 0))</f>
         <v>0</v>
       </c>
       <c r="N67" s="3">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v>8</v>
       </c>
       <c r="O67" s="38"/>
@@ -14743,12 +14782,12 @@
       <c r="EW67" s="38"/>
       <c r="EX67" s="38"/>
     </row>
-    <row r="68" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A68" s="12"/>
       <c r="B68" s="80" t="s">
         <v>167</v>
       </c>
-      <c r="C68" s="140" t="s">
+      <c r="C68" s="109" t="s">
         <v>58</v>
       </c>
       <c r="D68" s="80" t="s">
@@ -14778,12 +14817,12 @@
       <c r="L68" s="48">
         <v>45746</v>
       </c>
-      <c r="M68" s="148">
+      <c r="M68" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L68, H68&lt;1), -1, IF(H68=1, 1, 0))</f>
         <v>0</v>
       </c>
       <c r="N68" s="3">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v>17</v>
       </c>
       <c r="O68" s="38"/>
@@ -14927,10 +14966,10 @@
       <c r="EW68" s="38"/>
       <c r="EX68" s="38"/>
     </row>
-    <row r="69" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A69" s="11"/>
       <c r="B69" s="84"/>
-      <c r="C69" s="143" t="s">
+      <c r="C69" s="110" t="s">
         <v>38</v>
       </c>
       <c r="D69" s="84"/>
@@ -14942,9 +14981,9 @@
       <c r="J69" s="90"/>
       <c r="K69" s="87"/>
       <c r="L69" s="90"/>
-      <c r="M69" s="148"/>
+      <c r="M69" s="115"/>
       <c r="N69" s="3" t="str">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v/>
       </c>
       <c r="O69" s="51"/>
@@ -15088,12 +15127,12 @@
       <c r="EW69" s="51"/>
       <c r="EX69" s="51"/>
     </row>
-    <row r="70" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A70" s="11"/>
       <c r="B70" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="C70" s="144" t="s">
+      <c r="C70" s="111" t="s">
         <v>56</v>
       </c>
       <c r="D70" s="52" t="s">
@@ -15123,12 +15162,12 @@
       <c r="L70" s="55">
         <v>45833</v>
       </c>
-      <c r="M70" s="148">
+      <c r="M70" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L70, H70&lt;1), -1, IF(H70=1, 1, 0))</f>
         <v>0</v>
       </c>
       <c r="N70" s="3">
-        <f t="shared" ref="N70:N74" si="71">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="N70:N74" si="74">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>25</v>
       </c>
       <c r="O70" s="38"/>
@@ -15272,12 +15311,12 @@
       <c r="EW70" s="38"/>
       <c r="EX70" s="38"/>
     </row>
-    <row r="71" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A71" s="11"/>
       <c r="B71" s="52" t="s">
         <v>136</v>
       </c>
-      <c r="C71" s="144" t="s">
+      <c r="C71" s="111" t="s">
         <v>62</v>
       </c>
       <c r="D71" s="52" t="s">
@@ -15307,12 +15346,12 @@
       <c r="L71" s="55">
         <v>45818</v>
       </c>
-      <c r="M71" s="148">
+      <c r="M71" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L71, H71&lt;1), -1, IF(H71=1, 1, 0))</f>
         <v>0</v>
       </c>
       <c r="N71" s="3">
-        <f t="shared" si="71"/>
+        <f t="shared" si="74"/>
         <v>6</v>
       </c>
       <c r="O71" s="38"/>
@@ -15456,12 +15495,12 @@
       <c r="EW71" s="38"/>
       <c r="EX71" s="38"/>
     </row>
-    <row r="72" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A72" s="11"/>
       <c r="B72" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="C72" s="144" t="s">
+      <c r="C72" s="111" t="s">
         <v>109</v>
       </c>
       <c r="D72" s="52" t="s">
@@ -15491,12 +15530,12 @@
       <c r="L72" s="55">
         <v>45825</v>
       </c>
-      <c r="M72" s="148">
+      <c r="M72" s="115">
         <f ca="1">IF(AND(TODAY()&gt;L72, H72&lt;1), -1, IF(H72=1, 1, 0))</f>
         <v>0</v>
       </c>
       <c r="N72" s="3">
-        <f t="shared" si="71"/>
+        <f t="shared" si="74"/>
         <v>8</v>
       </c>
       <c r="O72" s="38"/>
@@ -15640,10 +15679,10 @@
       <c r="EW72" s="38"/>
       <c r="EX72" s="38"/>
     </row>
-    <row r="73" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A73" s="11"/>
       <c r="B73" s="56"/>
-      <c r="C73" s="145"/>
+      <c r="C73" s="112"/>
       <c r="D73" s="56"/>
       <c r="E73" s="56"/>
       <c r="F73" s="56"/>
@@ -15655,7 +15694,7 @@
       <c r="L73" s="59"/>
       <c r="M73" s="13"/>
       <c r="N73" s="3" t="str">
-        <f t="shared" si="71"/>
+        <f t="shared" si="74"/>
         <v/>
       </c>
       <c r="O73" s="32"/>
@@ -15799,10 +15838,10 @@
       <c r="EW73" s="32"/>
       <c r="EX73" s="32"/>
     </row>
-    <row r="74" spans="1:154" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:154" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A74" s="12"/>
       <c r="B74" s="60"/>
-      <c r="C74" s="146" t="s">
+      <c r="C74" s="113" t="s">
         <v>0</v>
       </c>
       <c r="D74" s="60"/>
@@ -15816,7 +15855,7 @@
       <c r="L74" s="64"/>
       <c r="M74" s="13"/>
       <c r="N74" s="4" t="str">
-        <f t="shared" si="71"/>
+        <f t="shared" si="74"/>
         <v/>
       </c>
       <c r="O74" s="65"/>
@@ -15961,13 +16000,45 @@
       <c r="EX74" s="65"/>
     </row>
   </sheetData>
-  <autoFilter ref="B5:M74" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C9:L16">
+  <autoFilter ref="B5:M74">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="ES"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="B20:M64">
+      <sortCondition ref="K5:K74"/>
+    </sortState>
+  </autoFilter>
+  <sortState ref="C9:L16">
     <sortCondition ref="H9:H16"/>
   </sortState>
   <mergeCells count="41">
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="W2:AF2"/>
+    <mergeCell ref="W1:AF1"/>
+    <mergeCell ref="O1:U1"/>
+    <mergeCell ref="O2:U2"/>
+    <mergeCell ref="BL4:BR4"/>
+    <mergeCell ref="O4:U4"/>
+    <mergeCell ref="V4:AB4"/>
+    <mergeCell ref="AC4:AI4"/>
+    <mergeCell ref="AJ4:AP4"/>
+    <mergeCell ref="AQ4:AW4"/>
+    <mergeCell ref="AX4:BD4"/>
+    <mergeCell ref="BE4:BK4"/>
     <mergeCell ref="EK4:EQ4"/>
     <mergeCell ref="ER4:EX4"/>
     <mergeCell ref="AG1:AM1"/>
@@ -15984,29 +16055,6 @@
     <mergeCell ref="CG4:CM4"/>
     <mergeCell ref="CN4:CT4"/>
     <mergeCell ref="CU4:DA4"/>
-    <mergeCell ref="BL4:BR4"/>
-    <mergeCell ref="O4:U4"/>
-    <mergeCell ref="V4:AB4"/>
-    <mergeCell ref="AC4:AI4"/>
-    <mergeCell ref="AJ4:AP4"/>
-    <mergeCell ref="AQ4:AW4"/>
-    <mergeCell ref="AX4:BD4"/>
-    <mergeCell ref="BE4:BK4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="W2:AF2"/>
-    <mergeCell ref="W1:AF1"/>
-    <mergeCell ref="O1:U1"/>
-    <mergeCell ref="O2:U2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <phoneticPr fontId="35" type="noConversion"/>
   <conditionalFormatting sqref="H7:H33 H36:H56 H58:H74">
@@ -16070,21 +16118,21 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="12">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="W2" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="12">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="W2">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a Project Schedule in this worksheet._x000a_Enter title of this project in cell B1. _x000a_Information on how to use this worksheet, including instructions for screen readers and the author of this workbook, is in the About worksheet._x000a_" sqref="A1:B1" xr:uid="{D005F8F4-EA16-4627-8A05-1997BE425B88}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Company name in cel B2." sqref="A2:B2" xr:uid="{75F274B0-5B30-4CC0-A53C-C012C0845179}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the name of the Project Lead in cell C3. Enter the Project Start date in cell Q1. Project Start: label is in cell I1." sqref="A3:B3" xr:uid="{EEA7C783-457F-401F-98B9-9035587B9210}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The Display week in cell Q2 is the starting week to display in the project schedule in cell I4. The project start date is Week 1. To change the display week, enter a new week number in cell Q2._x000a__x000a_Start date for each week is auto calculated starting in I4." sqref="A4:B4" xr:uid="{43382715-6BC7-4B19-A31B-4B13A11ED166}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cells I5 through BL5 contain the day number for the week represented in the cell block above each date and are auto calculated._x000a__x000a_Today's date is outlined from today's date in row 5 through the entire date column to the end of the project schedule." sqref="A5:A6 B5" xr:uid="{7A3789A6-A3FB-43B6-A4F7-8C0AC564F67E}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cell B8 contains the Phase 1 sample title. Enter a new title in cell B8._x000a_To delete the phase and work only from tasks, simply delete this row." sqref="A7:B7" xr:uid="{CEC78982-AFA8-419E-B0A2-676B709E5100}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="B9 contains the task name.  C9 is the assignee.  D9 is a progress bar that shades based on the number entered into the cell.  _x000a__x000a_E9 contains the start date and F9 contains the end date._x000a__x000a_The Gantt chart will fill in starting in cell I9 based on task dates." sqref="A8:B8 B10 B12 B14 B16:B17 B19 B21 B23 B25" xr:uid="{D870A2F6-6B07-4F5A-A81D-4BCCFADF8796}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Rows 10 through 13 repeat the pattern from row 9. _x000a__x000a_Repeat the instructions from cell A9 for all task rows in this worksheet. _x000a__x000a_Continue entering tasks in cells A10 through A13 or go to cell A14 to learn more." sqref="A9:B9 B11 B13 B15 B18 B20 B22 B24 B26" xr:uid="{872449A7-C3CC-45B6-BA90-B1AAD66BA0E5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cell B14 contains the Phase 2 sample title. Enter a new title in cell B14._x000a_To delete the phase and work only from tasks, simply delete this row. To remove the phase, simply delete the row. Add tasks to previous phase by entering a new row above this one._x000a_" sqref="A27:B27" xr:uid="{4F48FC41-E335-47F1-87AA-3333A52AD81C}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 3's sample block starts in cell B20." sqref="A69:B69" xr:uid="{956902D1-D3B5-416D-BB69-9362D193BC0A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A74:B74" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a Project Schedule in this worksheet._x000a_Enter title of this project in cell B1. _x000a_Information on how to use this worksheet, including instructions for screen readers and the author of this workbook, is in the About worksheet._x000a_" sqref="A1:B1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Company name in cel B2." sqref="A2:B2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the name of the Project Lead in cell C3. Enter the Project Start date in cell Q1. Project Start: label is in cell I1." sqref="A3:B3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The Display week in cell Q2 is the starting week to display in the project schedule in cell I4. The project start date is Week 1. To change the display week, enter a new week number in cell Q2._x000a__x000a_Start date for each week is auto calculated starting in I4." sqref="A4:B4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cells I5 through BL5 contain the day number for the week represented in the cell block above each date and are auto calculated._x000a__x000a_Today's date is outlined from today's date in row 5 through the entire date column to the end of the project schedule." sqref="A5:A6 B5"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cell B8 contains the Phase 1 sample title. Enter a new title in cell B8._x000a_To delete the phase and work only from tasks, simply delete this row." sqref="A7:B7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="B9 contains the task name.  C9 is the assignee.  D9 is a progress bar that shades based on the number entered into the cell.  _x000a__x000a_E9 contains the start date and F9 contains the end date._x000a__x000a_The Gantt chart will fill in starting in cell I9 based on task dates." sqref="A8:B8 B10 B12 B14 B16:B17 B19 B21 B23 B25"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Rows 10 through 13 repeat the pattern from row 9. _x000a__x000a_Repeat the instructions from cell A9 for all task rows in this worksheet. _x000a__x000a_Continue entering tasks in cells A10 through A13 or go to cell A14 to learn more." sqref="A9:B9 B11 B13 B15 B18 B20 B22 B24 B26"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cell B14 contains the Phase 2 sample title. Enter a new title in cell B14._x000a_To delete the phase and work only from tasks, simply delete this row. To remove the phase, simply delete the row. Add tasks to previous phase by entering a new row above this one._x000a_" sqref="A27:B27"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 3's sample block starts in cell B20." sqref="A69:B69"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A74:B74"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
@@ -16118,16 +16166,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78435F54-EC3A-3E43-A6C7-6CD96FCDDB61}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18">
       <c r="A1" s="77">
         <f>DATE(2025,3,29)</f>
         <v>45745</v>
@@ -16201,42 +16249,42 @@
         <v>45835</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="8:8">
       <c r="H17" s="77"/>
     </row>
   </sheetData>
@@ -16246,128 +16294,128 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="87" style="5" customWidth="1"/>
     <col min="2" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="2" spans="1:2" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1"/>
+    <row r="2" spans="1:2" s="7" customFormat="1" ht="15.75">
       <c r="A2" s="68" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" s="9" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="69"/>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" s="8" customFormat="1" ht="31" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" s="8" customFormat="1" ht="31.5">
       <c r="A4" s="70" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="74.25" customHeight="1">
       <c r="A5" s="71" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="26.25" customHeight="1">
       <c r="A6" s="70" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="5" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" s="5" customFormat="1" ht="204.95" customHeight="1">
       <c r="A7" s="72" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="8" customFormat="1" ht="31" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" s="8" customFormat="1" ht="31.5">
       <c r="A8" s="70" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" ht="57">
       <c r="A9" s="71" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="5" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" s="5" customFormat="1" ht="27.95" customHeight="1">
       <c r="A10" s="73" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="8" customFormat="1" ht="31" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" s="8" customFormat="1" ht="31.5">
       <c r="A11" s="70" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" ht="28.5">
       <c r="A12" s="71" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="5" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" s="5" customFormat="1" ht="27.95" customHeight="1">
       <c r="A13" s="73" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="8" customFormat="1" ht="31" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" s="8" customFormat="1" ht="31.5">
       <c r="A14" s="70" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" ht="75" customHeight="1">
       <c r="A15" s="71" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2" ht="71.25">
       <c r="A16" s="71" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1">
       <c r="A17" s="74"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1">
       <c r="A18" s="74"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1">
       <c r="A19" s="74"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:1">
       <c r="A20" s="74"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:1">
       <c r="A21" s="74" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:1">
       <c r="A22" s="74" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:1">
       <c r="A23" s="74"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:1">
       <c r="A24" s="74"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A13" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A10" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="A13" r:id="rId1"/>
+    <hyperlink ref="A10" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -16376,35 +16424,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16716,34 +16735,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16764,6 +16785,33 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>